<commit_message>
show card brief text
</commit_message>
<xml_diff>
--- a/reading/readings.xlsx
+++ b/reading/readings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -234,6 +234,10 @@
   </si>
   <si>
     <t>assets\thumb\framegraph_gdc2018.png</t>
+  </si>
+  <si>
+    <t>这是一些简单的介绍文字，不要太长，也不要太短，差不多就行了。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -352,7 +356,10 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -409,19 +416,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:K7" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:K7" totalsRowShown="0" headerRowDxfId="9">
   <tableColumns count="11">
-    <tableColumn id="1" name="title" dataDxfId="7"/>
-    <tableColumn id="8" name="author" dataDxfId="6"/>
-    <tableColumn id="11" name="type" dataDxfId="5"/>
-    <tableColumn id="10" name="homepage" dataDxfId="4"/>
-    <tableColumn id="2" name="date" dataDxfId="3"/>
+    <tableColumn id="1" name="title" dataDxfId="8"/>
+    <tableColumn id="8" name="author" dataDxfId="7"/>
+    <tableColumn id="11" name="type" dataDxfId="6"/>
+    <tableColumn id="10" name="homepage" dataDxfId="5"/>
+    <tableColumn id="2" name="date" dataDxfId="4"/>
     <tableColumn id="9" name="publisher"/>
-    <tableColumn id="3" name="tags" dataDxfId="2"/>
-    <tableColumn id="4" name="thumb" dataDxfId="1"/>
+    <tableColumn id="3" name="tags" dataDxfId="3"/>
+    <tableColumn id="4" name="thumb" dataDxfId="2"/>
     <tableColumn id="5" name="video"/>
-    <tableColumn id="6" name="url" dataDxfId="0"/>
-    <tableColumn id="7" name="brief"/>
+    <tableColumn id="6" name="url" dataDxfId="1"/>
+    <tableColumn id="7" name="brief" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -692,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -707,7 +714,7 @@
     <col min="8" max="8" width="18.375" style="1" customWidth="1"/>
     <col min="9" max="9" width="29.125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="27.875" customWidth="1"/>
+    <col min="11" max="11" width="27.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -741,7 +748,7 @@
       <c r="J1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -774,7 +781,7 @@
       <c r="J2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -809,7 +816,7 @@
       <c r="J3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -844,6 +851,9 @@
       <c r="J4" s="11" t="s">
         <v>40</v>
       </c>
+      <c r="K4" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -873,6 +883,9 @@
       <c r="J5" s="11" t="s">
         <v>41</v>
       </c>
+      <c r="K5" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="57" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -902,6 +915,9 @@
       <c r="J6" s="11" t="s">
         <v>42</v>
       </c>
+      <c r="K6" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -931,6 +947,9 @@
       <c r="I7" s="7"/>
       <c r="J7" s="11" t="s">
         <v>45</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add s2018 dxr intro ppt
</commit_message>
<xml_diff>
--- a/reading/readings.xlsx
+++ b/reading/readings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="132">
   <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -470,6 +470,52 @@
   </si>
   <si>
     <t>PBR 中广泛使用的Cook-Torrance BRDF是1982年此篇论文提出。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Introduction to DirectX Raytracing Shaders</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chris Wyman</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://intro-to-dxr.cwyman.org</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018年8月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIGGRAPH 2018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ray Tracing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>assets\thumb\intro_dxr_sig2018.png</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Q1cuuepVNoY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>assets\slides\s2018_IntroDXR_RaytracingShaders.pdf</t>
+  </si>
+  <si>
+    <t>https://neil3d.github.io/3dengine/DXRPreview.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://cwyman.org/code/dxrTutors/dxr_tutors.md.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Real-time Ray Tracing 无疑是2018年的热点，GDC 2018发布DXR API之后，SIGGRAPH这个专场值得一看。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -641,7 +687,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L12" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L13" totalsRowShown="0" headerRowDxfId="10">
   <tableColumns count="12">
     <tableColumn id="1" name="title" dataDxfId="9"/>
     <tableColumn id="8" name="author" dataDxfId="8"/>
@@ -923,11 +969,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1235,136 +1281,174 @@
     </row>
     <row r="9" spans="1:12" ht="57" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="57" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D10" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H10" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J10" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="K9" s="9"/>
-      <c r="L9" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>87</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="57" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="K11" s="9"/>
       <c r="L11" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="57" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>111</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>112</v>
+        <v>17</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>114</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>115</v>
+        <v>18</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>116</v>
+        <v>45</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>117</v>
+        <v>48</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>118</v>
+        <v>36</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K12" s="9"/>
       <c r="L12" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="K13" s="9"/>
+      <c r="L13" s="1" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1373,20 +1457,20 @@
   <hyperlinks>
     <hyperlink ref="H5" r:id="rId1"/>
     <hyperlink ref="C5" r:id="rId2"/>
-    <hyperlink ref="C11" r:id="rId3"/>
+    <hyperlink ref="C12" r:id="rId3"/>
     <hyperlink ref="H6" r:id="rId4"/>
     <hyperlink ref="I5" r:id="rId5"/>
-    <hyperlink ref="I11" r:id="rId6"/>
+    <hyperlink ref="I12" r:id="rId6"/>
     <hyperlink ref="I6" r:id="rId7"/>
-    <hyperlink ref="I9" r:id="rId8"/>
-    <hyperlink ref="C9" r:id="rId9"/>
+    <hyperlink ref="I10" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
     <hyperlink ref="G5" r:id="rId10"/>
-    <hyperlink ref="G11" r:id="rId11"/>
+    <hyperlink ref="G12" r:id="rId11"/>
     <hyperlink ref="G6" r:id="rId12"/>
-    <hyperlink ref="G9" r:id="rId13"/>
-    <hyperlink ref="C10" r:id="rId14"/>
-    <hyperlink ref="G10" r:id="rId15"/>
-    <hyperlink ref="I10" r:id="rId16"/>
+    <hyperlink ref="G10" r:id="rId13"/>
+    <hyperlink ref="C11" r:id="rId14"/>
+    <hyperlink ref="G11" r:id="rId15"/>
+    <hyperlink ref="I11" r:id="rId16"/>
     <hyperlink ref="H4" r:id="rId17"/>
     <hyperlink ref="C4" r:id="rId18"/>
     <hyperlink ref="G4" r:id="rId19"/>
@@ -1401,14 +1485,20 @@
     <hyperlink ref="I8" r:id="rId28"/>
     <hyperlink ref="J8" r:id="rId29"/>
     <hyperlink ref="K8" r:id="rId30"/>
-    <hyperlink ref="C12" r:id="rId31"/>
-    <hyperlink ref="G12" r:id="rId32"/>
-    <hyperlink ref="I12" r:id="rId33"/>
+    <hyperlink ref="C13" r:id="rId31"/>
+    <hyperlink ref="G13" r:id="rId32"/>
+    <hyperlink ref="I13" r:id="rId33"/>
+    <hyperlink ref="C9" r:id="rId34"/>
+    <hyperlink ref="G9" r:id="rId35"/>
+    <hyperlink ref="H9" r:id="rId36"/>
+    <hyperlink ref="I9" r:id="rId37"/>
+    <hyperlink ref="J9" r:id="rId38"/>
+    <hyperlink ref="K9" r:id="rId39"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId40"/>
   <tableParts count="1">
-    <tablePart r:id="rId35"/>
+    <tablePart r:id="rId41"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add ecs note link
</commit_message>
<xml_diff>
--- a/reading/readings.xlsx
+++ b/reading/readings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="134">
   <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -516,6 +516,14 @@
   </si>
   <si>
     <t>Real-time Ray Tracing 无疑是2018年的热点，GDC 2018发布DXR API之后，SIGGRAPH这个专场值得一看。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://gad.qq.com/article/detail/28682</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://neil3d.github.io/3dengine/why-ecs.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -973,7 +981,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1130,8 +1138,11 @@
       <c r="I4" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>85</v>
+      <c r="J4" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>132</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>70</v>
@@ -1494,11 +1505,13 @@
     <hyperlink ref="I9" r:id="rId37"/>
     <hyperlink ref="J9" r:id="rId38"/>
     <hyperlink ref="K9" r:id="rId39"/>
+    <hyperlink ref="K4" r:id="rId40"/>
+    <hyperlink ref="J4" r:id="rId41"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId40"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId42"/>
   <tableParts count="1">
-    <tablePart r:id="rId41"/>
+    <tablePart r:id="rId43"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add sig2012 disney pbs
</commit_message>
<xml_diff>
--- a/reading/readings.xlsx
+++ b/reading/readings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="143">
   <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -524,6 +524,39 @@
   </si>
   <si>
     <t>https://neil3d.github.io/3dengine/why-ecs.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Physically Based Shading at Disney</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brent Burley</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://blog.selfshadow.com/publications/s2012-shading-course/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIGGRAPH 2012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>assets\thumb\disney_pbs_sig2012.png</t>
+  </si>
+  <si>
+    <t>assets\slides\s2012_pbs_disney_brdf_slides_v2.pdf</t>
+  </si>
+  <si>
+    <t>assets\slides\s2012_pbs_disney_brdf_notes_v3.pdf</t>
+  </si>
+  <si>
+    <t>虚幻4的材质模型参考了迪士尼，这个演讲可以参考。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012年8月</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -695,7 +728,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L13" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L14" totalsRowShown="0" headerRowDxfId="10">
   <tableColumns count="12">
     <tableColumn id="1" name="title" dataDxfId="9"/>
     <tableColumn id="8" name="author" dataDxfId="8"/>
@@ -977,11 +1010,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1257,209 +1290,243 @@
     </row>
     <row r="8" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="E8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C9" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D9" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I9" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J9" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K9" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="57" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="E9" t="s">
-        <v>124</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="57" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="57" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C11" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D11" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H11" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J11" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="K10" s="9"/>
-      <c r="L10" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>87</v>
       </c>
       <c r="K11" s="9"/>
       <c r="L11" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="57" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="K12" s="9"/>
       <c r="L12" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="57" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>111</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>112</v>
+        <v>17</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>114</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>115</v>
+        <v>18</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>116</v>
+        <v>45</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>117</v>
+        <v>48</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>118</v>
+        <v>36</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="K14" s="9"/>
+      <c r="L14" s="1" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1468,20 +1535,20 @@
   <hyperlinks>
     <hyperlink ref="H5" r:id="rId1"/>
     <hyperlink ref="C5" r:id="rId2"/>
-    <hyperlink ref="C12" r:id="rId3"/>
+    <hyperlink ref="C13" r:id="rId3"/>
     <hyperlink ref="H6" r:id="rId4"/>
     <hyperlink ref="I5" r:id="rId5"/>
-    <hyperlink ref="I12" r:id="rId6"/>
+    <hyperlink ref="I13" r:id="rId6"/>
     <hyperlink ref="I6" r:id="rId7"/>
-    <hyperlink ref="I10" r:id="rId8"/>
-    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="I11" r:id="rId8"/>
+    <hyperlink ref="C11" r:id="rId9"/>
     <hyperlink ref="G5" r:id="rId10"/>
-    <hyperlink ref="G12" r:id="rId11"/>
+    <hyperlink ref="G13" r:id="rId11"/>
     <hyperlink ref="G6" r:id="rId12"/>
-    <hyperlink ref="G10" r:id="rId13"/>
-    <hyperlink ref="C11" r:id="rId14"/>
-    <hyperlink ref="G11" r:id="rId15"/>
-    <hyperlink ref="I11" r:id="rId16"/>
+    <hyperlink ref="G11" r:id="rId13"/>
+    <hyperlink ref="C12" r:id="rId14"/>
+    <hyperlink ref="G12" r:id="rId15"/>
+    <hyperlink ref="I12" r:id="rId16"/>
     <hyperlink ref="H4" r:id="rId17"/>
     <hyperlink ref="C4" r:id="rId18"/>
     <hyperlink ref="G4" r:id="rId19"/>
@@ -1491,27 +1558,31 @@
     <hyperlink ref="H7" r:id="rId23"/>
     <hyperlink ref="I7" r:id="rId24"/>
     <hyperlink ref="K7" r:id="rId25"/>
-    <hyperlink ref="C8" r:id="rId26"/>
-    <hyperlink ref="G8" r:id="rId27"/>
-    <hyperlink ref="I8" r:id="rId28"/>
-    <hyperlink ref="J8" r:id="rId29"/>
-    <hyperlink ref="K8" r:id="rId30"/>
-    <hyperlink ref="C13" r:id="rId31"/>
-    <hyperlink ref="G13" r:id="rId32"/>
-    <hyperlink ref="I13" r:id="rId33"/>
-    <hyperlink ref="C9" r:id="rId34"/>
-    <hyperlink ref="G9" r:id="rId35"/>
-    <hyperlink ref="H9" r:id="rId36"/>
-    <hyperlink ref="I9" r:id="rId37"/>
-    <hyperlink ref="J9" r:id="rId38"/>
-    <hyperlink ref="K9" r:id="rId39"/>
+    <hyperlink ref="C9" r:id="rId26"/>
+    <hyperlink ref="G9" r:id="rId27"/>
+    <hyperlink ref="I9" r:id="rId28"/>
+    <hyperlink ref="J9" r:id="rId29"/>
+    <hyperlink ref="K9" r:id="rId30"/>
+    <hyperlink ref="C14" r:id="rId31"/>
+    <hyperlink ref="G14" r:id="rId32"/>
+    <hyperlink ref="I14" r:id="rId33"/>
+    <hyperlink ref="C10" r:id="rId34"/>
+    <hyperlink ref="G10" r:id="rId35"/>
+    <hyperlink ref="H10" r:id="rId36"/>
+    <hyperlink ref="I10" r:id="rId37"/>
+    <hyperlink ref="J10" r:id="rId38"/>
+    <hyperlink ref="K10" r:id="rId39"/>
     <hyperlink ref="K4" r:id="rId40"/>
     <hyperlink ref="J4" r:id="rId41"/>
+    <hyperlink ref="C8" r:id="rId42"/>
+    <hyperlink ref="G8" r:id="rId43"/>
+    <hyperlink ref="I8" r:id="rId44"/>
+    <hyperlink ref="K8" r:id="rId45"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId42"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId46"/>
   <tableParts count="1">
-    <tablePart r:id="rId43"/>
+    <tablePart r:id="rId47"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
relative path for blog & notes
</commit_message>
<xml_diff>
--- a/reading/readings.xlsx
+++ b/reading/readings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="141">
   <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -346,16 +346,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://neil3d.github.io/3dengine/why-ecs.html</t>
-  </si>
-  <si>
-    <t>https://neil3d.github.io/3dengine/why-ecs.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://neil3d.github.io/unreal/pbr-theory.html</t>
-  </si>
-  <si>
     <t>https://www.bilibili.com/video/av10595011/</t>
   </si>
   <si>
@@ -428,10 +418,6 @@
     <t>assets\slides\s2013_pbs_epic_slides.pdf</t>
   </si>
   <si>
-    <t>https://neil3d.github.io/unreal/pbr-ue4.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>assets\slides\s2013_pbs_epic_notes_v2.pdf</t>
   </si>
   <si>
@@ -507,10 +493,6 @@
     <t>assets\slides\s2018_IntroDXR_RaytracingShaders.pdf</t>
   </si>
   <si>
-    <t>https://neil3d.github.io/3dengine/DXRPreview.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://cwyman.org/code/dxrTutors/dxr_tutors.md.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -523,10 +505,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://neil3d.github.io/3dengine/why-ecs.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Physically Based Shading at Disney</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -558,6 +536,18 @@
   <si>
     <t>2012年8月</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/3dengine/why-ecs.html</t>
+  </si>
+  <si>
+    <t>/unreal/pbr-theory.html</t>
+  </si>
+  <si>
+    <t>/unreal/pbr-ue4.html</t>
+  </si>
+  <si>
+    <t>/3dengine/DXRPreview.html</t>
   </si>
 </sst>
 </file>
@@ -1013,8 +1003,8 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1172,10 +1162,10 @@
         <v>78</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>70</v>
@@ -1210,11 +1200,11 @@
         <v>35</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>86</v>
+        <v>137</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="57" x14ac:dyDescent="0.2">
@@ -1243,7 +1233,7 @@
         <v>37</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="1" t="s">
@@ -1252,147 +1242,147 @@
     </row>
     <row r="7" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="E7" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="F7" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="G7" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H7" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="I7" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="J7" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="K7" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="L7" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>142</v>
-      </c>
       <c r="E8" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="9" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="12" t="s">
+      <c r="G9" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E9" t="s">
+      <c r="I9" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="J9" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="K9" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="L9" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="57" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" t="s">
         <v>120</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="H10" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="E10" t="s">
+      <c r="I10" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="J10" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="K10" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="L10" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="57" x14ac:dyDescent="0.2">
@@ -1418,13 +1408,13 @@
         <v>50</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>40</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="K11" s="9"/>
       <c r="L11" s="1" t="s">
@@ -1457,7 +1447,7 @@
         <v>66</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>87</v>
+        <v>138</v>
       </c>
       <c r="K12" s="9"/>
       <c r="L12" s="1" t="s">
@@ -1490,7 +1480,7 @@
         <v>36</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="1" t="s">
@@ -1499,35 +1489,35 @@
     </row>
     <row r="14" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" t="s">
         <v>111</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="G14" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="I14" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="E14" t="s">
-        <v>115</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>118</v>
-      </c>
       <c r="J14" s="9" t="s">
-        <v>87</v>
+        <v>138</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1552,7 +1542,7 @@
     <hyperlink ref="H4" r:id="rId17"/>
     <hyperlink ref="C4" r:id="rId18"/>
     <hyperlink ref="G4" r:id="rId19"/>
-    <hyperlink ref="J5" r:id="rId20"/>
+    <hyperlink ref="J5" r:id="rId20" display="https://neil3d.github.io/3dengine/why-ecs.html"/>
     <hyperlink ref="C7" r:id="rId21"/>
     <hyperlink ref="G7" r:id="rId22"/>
     <hyperlink ref="H7" r:id="rId23"/>
@@ -1561,7 +1551,7 @@
     <hyperlink ref="C9" r:id="rId26"/>
     <hyperlink ref="G9" r:id="rId27"/>
     <hyperlink ref="I9" r:id="rId28"/>
-    <hyperlink ref="J9" r:id="rId29"/>
+    <hyperlink ref="J9" r:id="rId29" display="https://neil3d.github.io/unreal/pbr-ue4.html"/>
     <hyperlink ref="K9" r:id="rId30"/>
     <hyperlink ref="C14" r:id="rId31"/>
     <hyperlink ref="G14" r:id="rId32"/>
@@ -1570,10 +1560,10 @@
     <hyperlink ref="G10" r:id="rId35"/>
     <hyperlink ref="H10" r:id="rId36"/>
     <hyperlink ref="I10" r:id="rId37"/>
-    <hyperlink ref="J10" r:id="rId38"/>
+    <hyperlink ref="J10" r:id="rId38" display="https://neil3d.github.io/3dengine/DXRPreview.html"/>
     <hyperlink ref="K10" r:id="rId39"/>
     <hyperlink ref="K4" r:id="rId40"/>
-    <hyperlink ref="J4" r:id="rId41"/>
+    <hyperlink ref="J4" r:id="rId41" display="https://neil3d.github.io/3dengine/why-ecs.html"/>
     <hyperlink ref="C8" r:id="rId42"/>
     <hyperlink ref="G8" r:id="rId43"/>
     <hyperlink ref="I8" r:id="rId44"/>

</xml_diff>

<commit_message>
add old cg papers
</commit_message>
<xml_diff>
--- a/reading/readings.xlsx
+++ b/reading/readings.xlsx
@@ -1,17 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neil/work/pages/reading/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="d">Sheet1!$L$16</definedName>
+    <definedName name="ha">Sheet1!$L$16</definedName>
+  </definedNames>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="165">
   <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -161,15 +176,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>assets\slides\oop_is_dead_long_live_dataoriented_design__stoyan_nikolov__cppcon_2018.pdf</t>
-  </si>
-  <si>
-    <t>assets\slides\Introduction_to_Data-Oriented_Design_2014DICE.pdf</t>
-  </si>
-  <si>
-    <t>assets\slides\Data-Oriented Design and C++ - Mike Acton - CppCon 2014.pptx</t>
-  </si>
-  <si>
     <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -178,9 +184,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>assets\slides\GDC17-framegraph.pptx</t>
-  </si>
-  <si>
     <t>Yuriy O’Donnell</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -205,18 +208,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>assets\thumb\oop_is_dead_cppcon2018.png</t>
-  </si>
-  <si>
-    <t>assets\thumb\dod_dice.png</t>
-  </si>
-  <si>
-    <t>assets\thumb\dod_cppcon2014.png</t>
-  </si>
-  <si>
-    <t>assets\thumb\framegraph_gdc2018.png</t>
-  </si>
-  <si>
     <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -265,16 +256,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>图形学理论</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>assets\thumb\the_rendering_equation.png</t>
-  </si>
-  <si>
-    <t>assets\paper\p143-kajiya.pdf</t>
-  </si>
-  <si>
     <t>在SIGGRAPH提出渲染方程的论文。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -307,9 +288,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>assets\thumb\overwatch_ecs_gdc2017.png</t>
-  </si>
-  <si>
     <t>Timothy Ford</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -369,19 +347,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>assets\thumb\pbr_background_sig2013.png</t>
-  </si>
-  <si>
     <t>https://youtu.be/j-A0mwsJRmk</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>assets\slides\s2013_pbs_physics_math_slides.pdf</t>
-  </si>
-  <si>
-    <t>assets\slides\s2013_pbs_physics_math_notes.pdf</t>
-  </si>
-  <si>
     <t>这个演讲的内容应作为UE4 PBR相关或其他演讲的背景资料，先行研读。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -408,15 +377,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>assets\thumb\ue4_pbr_sig2013.png</t>
-  </si>
-  <si>
-    <t>assets\slides\s2013_pbs_epic_slides.pdf</t>
-  </si>
-  <si>
-    <t>assets\slides\s2013_pbs_epic_notes_v2.pdf</t>
-  </si>
-  <si>
     <t>详细讲解了虚幻4中实现PBR的原理，重点是Split Sum Approximation。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -441,16 +401,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>图形学理论|PBR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>assets\thumb\cook-brdf.png</t>
-  </si>
-  <si>
-    <t>assets\paper\p7-cook.pdf</t>
-  </si>
-  <si>
     <t>PBR 中广泛使用的Cook-Torrance BRDF是1982年此篇论文提出。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -479,16 +429,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>assets\thumb\intro_dxr_sig2018.png</t>
-  </si>
-  <si>
     <t>https://youtu.be/Q1cuuepVNoY</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>assets\slides\s2018_IntroDXR_RaytracingShaders.pdf</t>
-  </si>
-  <si>
     <t>http://cwyman.org/code/dxrTutors/dxr_tutors.md.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -517,15 +461,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>assets\thumb\disney_pbs_sig2012.png</t>
-  </si>
-  <si>
-    <t>assets\slides\s2012_pbs_disney_brdf_slides_v2.pdf</t>
-  </si>
-  <si>
-    <t>assets\slides\s2012_pbs_disney_brdf_notes_v3.pdf</t>
-  </si>
-  <si>
     <t>虚幻4的材质模型参考了迪士尼，这个演讲可以参考。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -548,23 +483,174 @@
   <si>
     <t>广受关注的一个演讲，作者分享了《守望先锋》使用ECS架构的成功经验，但ECS的要点不止于此。</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MODELS OF LIQrHT REFLECTION
+FOR CO1PUTER SYNTHESIZED PICTURES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> James F. Blinn</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/citation.cfm?id=563893</t>
+  </si>
+  <si>
+    <t>1977年7月</t>
+  </si>
+  <si>
+    <t>ACM</t>
+  </si>
+  <si>
+    <t>图形学|PBR</t>
+  </si>
+  <si>
+    <t>图形学</t>
+  </si>
+  <si>
+    <t>assets/thumb/blinn.png</t>
+  </si>
+  <si>
+    <t>assets/paper/p192-blinn.pdf</t>
+  </si>
+  <si>
+    <t>经典的Blinn-Phong光照模型</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CASTING CURVED SHADOWS ON CURVED SURFACES </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lance William</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/citation.cfm?id=807402</t>
+  </si>
+  <si>
+    <t>1978年8月</t>
+  </si>
+  <si>
+    <t>assets/paper/p270-williams.pdf</t>
+  </si>
+  <si>
+    <t>/3dengine/shadow-mapping.html</t>
+  </si>
+  <si>
+    <t>Shadow Mapping</t>
+  </si>
+  <si>
+    <t>SIGGRAPH 1978</t>
+  </si>
+  <si>
+    <t>Shadow algorithms for computer graphics</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Franklin C. Crow</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/citation.cfm?id=563901</t>
+  </si>
+  <si>
+    <t>SIGGRAPH 1977</t>
+  </si>
+  <si>
+    <t>assets/paper/p242-crow.pdf</t>
+  </si>
+  <si>
+    <t>卡马克在DOOM3中所使用的Shadow Volume算法</t>
+  </si>
+  <si>
+    <t>assets/thumb/shadow_mapping.png</t>
+  </si>
+  <si>
+    <t>assets/thumb/shadow_volume.png</t>
+  </si>
+  <si>
+    <t>assets/thumb/oop_is_dead_cppcon2018.png</t>
+  </si>
+  <si>
+    <t>assets/slides/oop_is_dead_long_live_dataoriented_design__stoyan_nikolov__cppcon_2018.pdf</t>
+  </si>
+  <si>
+    <t>assets/thumb/dod_cppcon2014.png</t>
+  </si>
+  <si>
+    <t>assets/slides/Data-Oriented Design and C++ - Mike Acton - CppCon 2014.pptx</t>
+  </si>
+  <si>
+    <t>assets/thumb/pbr_background_sig2013.png</t>
+  </si>
+  <si>
+    <t>assets/slides/s2013_pbs_physics_math_slides.pdf</t>
+  </si>
+  <si>
+    <t>assets/slides/s2013_pbs_physics_math_notes.pdf</t>
+  </si>
+  <si>
+    <t>assets/thumb/disney_pbs_sig2012.png</t>
+  </si>
+  <si>
+    <t>assets/slides/s2012_pbs_disney_brdf_slides_v2.pdf</t>
+  </si>
+  <si>
+    <t>assets/slides/s2012_pbs_disney_brdf_notes_v3.pdf</t>
+  </si>
+  <si>
+    <t>assets/thumb/ue4_pbr_sig2013.png</t>
+  </si>
+  <si>
+    <t>assets/slides/s2013_pbs_epic_slides.pdf</t>
+  </si>
+  <si>
+    <t>assets/slides/s2013_pbs_epic_notes_v2.pdf</t>
+  </si>
+  <si>
+    <t>assets/thumb/intro_dxr_sig2018.png</t>
+  </si>
+  <si>
+    <t>assets/slides/s2018_IntroDXR_RaytracingShaders.pdf</t>
+  </si>
+  <si>
+    <t>assets/thumb/framegraph_gdc2018.png</t>
+  </si>
+  <si>
+    <t>assets/slides/GDC17-framegraph.pptx</t>
+  </si>
+  <si>
+    <t>assets/thumb/overwatch_ecs_gdc2017.png</t>
+  </si>
+  <si>
+    <t>assets/thumb/the_rendering_equation.png</t>
+  </si>
+  <si>
+    <t>assets/paper/p143-kajiya.pdf</t>
+  </si>
+  <si>
+    <t>assets/thumb/dod_dice.png</t>
+  </si>
+  <si>
+    <t>assets/slides/Introduction_to_Data-Oriented_Design_2014DICE.pdf</t>
+  </si>
+  <si>
+    <t>assets/thumb/cook-brdf.png</t>
+  </si>
+  <si>
+    <t>assets/paper/p7-cook.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -573,7 +659,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -582,7 +668,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -591,7 +677,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -653,8 +739,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -718,7 +804,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L14" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L17" totalsRowShown="0" headerRowDxfId="10">
   <tableColumns count="12">
     <tableColumn id="1" name="title" dataDxfId="9"/>
     <tableColumn id="8" name="author" dataDxfId="8"/>
@@ -729,8 +815,8 @@
     <tableColumn id="4" name="thumb" dataDxfId="4"/>
     <tableColumn id="5" name="video"/>
     <tableColumn id="6" name="url" dataDxfId="3"/>
-    <tableColumn id="11" name="my_blog" dataDxfId="2" dataCellStyle="超链接"/>
-    <tableColumn id="12" name="notes" dataDxfId="1" dataCellStyle="超链接"/>
+    <tableColumn id="11" name="my_blog" dataDxfId="2"/>
+    <tableColumn id="12" name="notes" dataDxfId="1"/>
     <tableColumn id="7" name="brief" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1000,26 +1086,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="23.75" style="1" customWidth="1"/>
+    <col min="1" max="3" width="23.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="12" customWidth="1"/>
-    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="29.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="20.625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="27.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="20.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="27.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1030,7 +1116,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>10</v>
@@ -1045,13 +1131,13 @@
         <v>3</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>4</v>
@@ -1065,10 +1151,10 @@
         <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>9</v>
@@ -1086,10 +1172,10 @@
         <v>5</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>6</v>
@@ -1124,16 +1210,16 @@
         <v>33</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="57" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -1144,7 +1230,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -1153,23 +1239,23 @@
         <v>23</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>47</v>
+        <v>141</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>35</v>
+        <v>142</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="1" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1177,7 +1263,7 @@
         <v>24</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
@@ -1186,275 +1272,275 @@
         <v>23</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>49</v>
+        <v>143</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>37</v>
+        <v>144</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>93</v>
+        <v>146</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>94</v>
+        <v>147</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E7" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="9" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" t="s">
         <v>98</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="12" t="s">
+      <c r="F9" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G9" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="I9" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="K9" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="L9" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>105</v>
-      </c>
     </row>
-    <row r="9" spans="1:12" ht="57" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="E9" t="s">
-        <v>119</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="57" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="G10" s="9" t="s">
-        <v>50</v>
+        <v>156</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>40</v>
+        <v>157</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="57" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>62</v>
-      </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>64</v>
+        <v>121</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>65</v>
+        <v>159</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>66</v>
+        <v>160</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="K12" s="9"/>
       <c r="L12" s="1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="57" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -1465,59 +1551,149 @@
         <v>16</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>48</v>
+        <v>161</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>36</v>
+        <v>162</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="E14" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="J14" s="9" t="s">
         <v>111</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>137</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="1" t="s">
-        <v>114</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" t="s">
+        <v>132</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" t="s">
+        <v>136</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1527,52 +1703,59 @@
     <hyperlink ref="C4" r:id="rId2"/>
     <hyperlink ref="C13" r:id="rId3"/>
     <hyperlink ref="H5" r:id="rId4"/>
-    <hyperlink ref="I4" r:id="rId5"/>
-    <hyperlink ref="I13" r:id="rId6"/>
-    <hyperlink ref="I5" r:id="rId7"/>
-    <hyperlink ref="I10" r:id="rId8"/>
+    <hyperlink ref="I4" r:id="rId5" display="assets\slides\oop_is_dead_long_live_dataoriented_design__stoyan_nikolov__cppcon_2018.pdf"/>
+    <hyperlink ref="I13" r:id="rId6" display="assets\slides\Introduction_to_Data-Oriented_Design_2014DICE.pdf"/>
+    <hyperlink ref="I5" r:id="rId7" display="assets\slides\Data-Oriented Design and C++ - Mike Acton - CppCon 2014.pptx"/>
+    <hyperlink ref="I10" r:id="rId8" display="assets\slides\GDC17-framegraph.pptx"/>
     <hyperlink ref="C10" r:id="rId9"/>
-    <hyperlink ref="G4" r:id="rId10"/>
-    <hyperlink ref="G13" r:id="rId11"/>
-    <hyperlink ref="G5" r:id="rId12"/>
-    <hyperlink ref="G10" r:id="rId13"/>
+    <hyperlink ref="G4" r:id="rId10" display="assets\thumb\oop_is_dead_cppcon2018.png"/>
+    <hyperlink ref="G13" r:id="rId11" display="assets\thumb\dod_dice.png"/>
+    <hyperlink ref="G5" r:id="rId12" display="assets\thumb\dod_cppcon2014.png"/>
+    <hyperlink ref="G10" r:id="rId13" display="assets\thumb\framegraph_gdc2018.png"/>
     <hyperlink ref="C12" r:id="rId14"/>
-    <hyperlink ref="G12" r:id="rId15"/>
-    <hyperlink ref="I12" r:id="rId16"/>
+    <hyperlink ref="G12" r:id="rId15" display="assets\thumb\the_rendering_equation.png"/>
+    <hyperlink ref="I12" r:id="rId16" display="assets\paper\p143-kajiya.pdf"/>
     <hyperlink ref="H11" r:id="rId17"/>
     <hyperlink ref="C11" r:id="rId18"/>
-    <hyperlink ref="G11" r:id="rId19"/>
+    <hyperlink ref="G11" r:id="rId19" display="assets\thumb\overwatch_ecs_gdc2017.png"/>
     <hyperlink ref="J4" r:id="rId20" display="https://neil3d.github.io/3dengine/why-ecs.html"/>
     <hyperlink ref="C6" r:id="rId21"/>
-    <hyperlink ref="G6" r:id="rId22"/>
+    <hyperlink ref="G6" r:id="rId22" display="assets\thumb\pbr_background_sig2013.png"/>
     <hyperlink ref="H6" r:id="rId23"/>
-    <hyperlink ref="I6" r:id="rId24"/>
-    <hyperlink ref="K6" r:id="rId25"/>
+    <hyperlink ref="I6" r:id="rId24" display="assets\slides\s2013_pbs_physics_math_slides.pdf"/>
+    <hyperlink ref="K6" r:id="rId25" display="assets\slides\s2013_pbs_physics_math_notes.pdf"/>
     <hyperlink ref="C8" r:id="rId26"/>
-    <hyperlink ref="G8" r:id="rId27"/>
-    <hyperlink ref="I8" r:id="rId28"/>
+    <hyperlink ref="G8" r:id="rId27" display="assets\thumb\ue4_pbr_sig2013.png"/>
+    <hyperlink ref="I8" r:id="rId28" display="assets\slides\s2013_pbs_epic_slides.pdf"/>
     <hyperlink ref="J8" r:id="rId29" display="https://neil3d.github.io/unreal/pbr-ue4.html"/>
-    <hyperlink ref="K8" r:id="rId30"/>
+    <hyperlink ref="K8" r:id="rId30" display="assets\slides\s2013_pbs_epic_notes_v2.pdf"/>
     <hyperlink ref="C14" r:id="rId31"/>
-    <hyperlink ref="G14" r:id="rId32"/>
-    <hyperlink ref="I14" r:id="rId33"/>
+    <hyperlink ref="G14" r:id="rId32" display="assets\thumb\cook-brdf.png"/>
+    <hyperlink ref="I14" r:id="rId33" display="assets\paper\p7-cook.pdf"/>
     <hyperlink ref="C9" r:id="rId34"/>
-    <hyperlink ref="G9" r:id="rId35"/>
+    <hyperlink ref="G9" r:id="rId35" display="assets\thumb\intro_dxr_sig2018.png"/>
     <hyperlink ref="H9" r:id="rId36"/>
-    <hyperlink ref="I9" r:id="rId37"/>
+    <hyperlink ref="I9" r:id="rId37" display="assets\slides\s2018_IntroDXR_RaytracingShaders.pdf"/>
     <hyperlink ref="J9" r:id="rId38" display="https://neil3d.github.io/3dengine/DXRPreview.html"/>
     <hyperlink ref="K9" r:id="rId39"/>
     <hyperlink ref="K11" r:id="rId40"/>
     <hyperlink ref="J11" r:id="rId41" display="https://neil3d.github.io/3dengine/why-ecs.html"/>
     <hyperlink ref="C7" r:id="rId42"/>
-    <hyperlink ref="G7" r:id="rId43"/>
-    <hyperlink ref="I7" r:id="rId44"/>
-    <hyperlink ref="K7" r:id="rId45"/>
+    <hyperlink ref="G7" r:id="rId43" display="assets\thumb\disney_pbs_sig2012.png"/>
+    <hyperlink ref="I7" r:id="rId44" display="assets\slides\s2012_pbs_disney_brdf_slides_v2.pdf"/>
+    <hyperlink ref="K7" r:id="rId45" display="assets\slides\s2012_pbs_disney_brdf_notes_v3.pdf"/>
+    <hyperlink ref="G15" r:id="rId46"/>
+    <hyperlink ref="I15" r:id="rId47"/>
+    <hyperlink ref="I16" r:id="rId48"/>
+    <hyperlink ref="C17" r:id="rId49"/>
+    <hyperlink ref="I17" r:id="rId50"/>
+    <hyperlink ref="G16" r:id="rId51"/>
+    <hyperlink ref="G17" r:id="rId52"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId46"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId53"/>
   <tableParts count="1">
-    <tablePart r:id="rId47"/>
+    <tablePart r:id="rId54"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add Scott Meyers talk on Cpu Caches
</commit_message>
<xml_diff>
--- a/reading/readings.xlsx
+++ b/reading/readings.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="d">Sheet1!$L$16</definedName>
-    <definedName name="ha">Sheet1!$L$16</definedName>
+    <definedName name="d">Sheet1!$L$17</definedName>
+    <definedName name="ha">Sheet1!$L$17</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="174">
   <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -633,6 +633,33 @@
   </si>
   <si>
     <t xml:space="preserve">Casting curved shadows on curved surfaces </t>
+  </si>
+  <si>
+    <t>Scott Meyers</t>
+  </si>
+  <si>
+    <t>Cpu Caches and Why You Care</t>
+  </si>
+  <si>
+    <t>https://www.aristeia.com</t>
+  </si>
+  <si>
+    <t>2014年11月</t>
+  </si>
+  <si>
+    <t>code::dive</t>
+  </si>
+  <si>
+    <t>assets/thumb/scott_cpu_cache.png</t>
+  </si>
+  <si>
+    <t>https://youtu.be/WDIkqP4JbkE</t>
+  </si>
+  <si>
+    <t>assets/slides/codedive-CPUCachesHandouts.pdf</t>
+  </si>
+  <si>
+    <t>《Effective C++》看过吧，那你必须看看 这个演讲，犀利，洗脑！Scott Meyers 依然给力！</t>
   </si>
 </sst>
 </file>
@@ -803,7 +830,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L17" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L18" totalsRowShown="0" headerRowDxfId="10">
   <tableColumns count="12">
     <tableColumn id="1" name="title" dataDxfId="9"/>
     <tableColumn id="8" name="author" dataDxfId="8"/>
@@ -1085,11 +1112,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1287,411 +1314,445 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>73</v>
+        <v>166</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>165</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>75</v>
+        <v>167</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" t="s">
-        <v>77</v>
+        <v>168</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>79</v>
+        <v>171</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>145</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
       <c r="L6" s="1" t="s">
-        <v>80</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>78</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="H7" s="7"/>
+        <v>143</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="I7" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="J7" s="9"/>
+        <v>144</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>111</v>
+      </c>
       <c r="K7" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C9" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D9" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I9" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J9" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K9" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:12" ht="75" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D10" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>98</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H10" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I10" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J10" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K10" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C11" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D11" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H11" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I11" s="9" t="s">
         <v>155</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="K10" s="9"/>
-      <c r="L10" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="K11" s="9"/>
+      <c r="L11" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="K12" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C13" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D13" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G13" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I13" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="J13" s="9" t="s">
         <v>111</v>
-      </c>
-      <c r="K12" s="9"/>
-      <c r="L12" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="60" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>110</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>119</v>
+        <v>41</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="K15" s="9"/>
+      <c r="L15" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D16" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>118</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E16" t="s">
-        <v>130</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>131</v>
+        <v>164</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="E17" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G17" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" t="s">
+        <v>134</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I18" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>136</v>
       </c>
     </row>
@@ -1700,61 +1761,65 @@
   <hyperlinks>
     <hyperlink ref="H4" r:id="rId1"/>
     <hyperlink ref="C4" r:id="rId2"/>
-    <hyperlink ref="C13" r:id="rId3"/>
+    <hyperlink ref="C14" r:id="rId3"/>
     <hyperlink ref="H5" r:id="rId4"/>
     <hyperlink ref="I4" r:id="rId5" display="assets\slides\oop_is_dead_long_live_dataoriented_design__stoyan_nikolov__cppcon_2018.pdf"/>
-    <hyperlink ref="I13" r:id="rId6" display="assets\slides\Introduction_to_Data-Oriented_Design_2014DICE.pdf"/>
+    <hyperlink ref="I14" r:id="rId6" display="assets\slides\Introduction_to_Data-Oriented_Design_2014DICE.pdf"/>
     <hyperlink ref="I5" r:id="rId7" display="assets\slides\Data-Oriented Design and C++ - Mike Acton - CppCon 2014.pptx"/>
-    <hyperlink ref="I10" r:id="rId8" display="assets\slides\GDC17-framegraph.pptx"/>
-    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="I11" r:id="rId8" display="assets\slides\GDC17-framegraph.pptx"/>
+    <hyperlink ref="C11" r:id="rId9"/>
     <hyperlink ref="G4" r:id="rId10" display="assets\thumb\oop_is_dead_cppcon2018.png"/>
-    <hyperlink ref="G13" r:id="rId11" display="assets\thumb\dod_dice.png"/>
+    <hyperlink ref="G14" r:id="rId11" display="assets\thumb\dod_dice.png"/>
     <hyperlink ref="G5" r:id="rId12" display="assets\thumb\dod_cppcon2014.png"/>
-    <hyperlink ref="G10" r:id="rId13" display="assets\thumb\framegraph_gdc2018.png"/>
-    <hyperlink ref="C12" r:id="rId14"/>
-    <hyperlink ref="G12" r:id="rId15" display="assets\thumb\the_rendering_equation.png"/>
-    <hyperlink ref="I12" r:id="rId16" display="assets\paper\p143-kajiya.pdf"/>
-    <hyperlink ref="H11" r:id="rId17"/>
-    <hyperlink ref="C11" r:id="rId18"/>
-    <hyperlink ref="G11" r:id="rId19" display="assets\thumb\overwatch_ecs_gdc2017.png"/>
+    <hyperlink ref="G11" r:id="rId13" display="assets\thumb\framegraph_gdc2018.png"/>
+    <hyperlink ref="C13" r:id="rId14"/>
+    <hyperlink ref="G13" r:id="rId15" display="assets\thumb\the_rendering_equation.png"/>
+    <hyperlink ref="I13" r:id="rId16" display="assets\paper\p143-kajiya.pdf"/>
+    <hyperlink ref="H12" r:id="rId17"/>
+    <hyperlink ref="C12" r:id="rId18"/>
+    <hyperlink ref="G12" r:id="rId19" display="assets\thumb\overwatch_ecs_gdc2017.png"/>
     <hyperlink ref="J4" r:id="rId20" display="https://neil3d.github.io/3dengine/why-ecs.html"/>
-    <hyperlink ref="C6" r:id="rId21"/>
-    <hyperlink ref="G6" r:id="rId22" display="assets\thumb\pbr_background_sig2013.png"/>
-    <hyperlink ref="H6" r:id="rId23"/>
-    <hyperlink ref="I6" r:id="rId24" display="assets\slides\s2013_pbs_physics_math_slides.pdf"/>
-    <hyperlink ref="K6" r:id="rId25" display="assets\slides\s2013_pbs_physics_math_notes.pdf"/>
-    <hyperlink ref="C8" r:id="rId26"/>
-    <hyperlink ref="G8" r:id="rId27" display="assets\thumb\ue4_pbr_sig2013.png"/>
-    <hyperlink ref="I8" r:id="rId28" display="assets\slides\s2013_pbs_epic_slides.pdf"/>
-    <hyperlink ref="J8" r:id="rId29" display="https://neil3d.github.io/unreal/pbr-ue4.html"/>
-    <hyperlink ref="K8" r:id="rId30" display="assets\slides\s2013_pbs_epic_notes_v2.pdf"/>
-    <hyperlink ref="C14" r:id="rId31"/>
-    <hyperlink ref="G14" r:id="rId32" display="assets\thumb\cook-brdf.png"/>
-    <hyperlink ref="I14" r:id="rId33" display="assets\paper\p7-cook.pdf"/>
-    <hyperlink ref="C9" r:id="rId34"/>
-    <hyperlink ref="G9" r:id="rId35" display="assets\thumb\intro_dxr_sig2018.png"/>
-    <hyperlink ref="H9" r:id="rId36"/>
-    <hyperlink ref="I9" r:id="rId37" display="assets\slides\s2018_IntroDXR_RaytracingShaders.pdf"/>
-    <hyperlink ref="J9" r:id="rId38" display="https://neil3d.github.io/3dengine/DXRPreview.html"/>
-    <hyperlink ref="K9" r:id="rId39"/>
-    <hyperlink ref="K11" r:id="rId40"/>
-    <hyperlink ref="J11" r:id="rId41" display="https://neil3d.github.io/3dengine/why-ecs.html"/>
-    <hyperlink ref="C7" r:id="rId42"/>
-    <hyperlink ref="G7" r:id="rId43" display="assets\thumb\disney_pbs_sig2012.png"/>
-    <hyperlink ref="I7" r:id="rId44" display="assets\slides\s2012_pbs_disney_brdf_slides_v2.pdf"/>
-    <hyperlink ref="K7" r:id="rId45" display="assets\slides\s2012_pbs_disney_brdf_notes_v3.pdf"/>
-    <hyperlink ref="G15" r:id="rId46"/>
-    <hyperlink ref="I15" r:id="rId47"/>
-    <hyperlink ref="I16" r:id="rId48"/>
-    <hyperlink ref="C17" r:id="rId49"/>
-    <hyperlink ref="I17" r:id="rId50"/>
-    <hyperlink ref="G16" r:id="rId51"/>
-    <hyperlink ref="G17" r:id="rId52"/>
+    <hyperlink ref="C7" r:id="rId21"/>
+    <hyperlink ref="G7" r:id="rId22" display="assets\thumb\pbr_background_sig2013.png"/>
+    <hyperlink ref="H7" r:id="rId23"/>
+    <hyperlink ref="I7" r:id="rId24" display="assets\slides\s2013_pbs_physics_math_slides.pdf"/>
+    <hyperlink ref="K7" r:id="rId25" display="assets\slides\s2013_pbs_physics_math_notes.pdf"/>
+    <hyperlink ref="C9" r:id="rId26"/>
+    <hyperlink ref="G9" r:id="rId27" display="assets\thumb\ue4_pbr_sig2013.png"/>
+    <hyperlink ref="I9" r:id="rId28" display="assets\slides\s2013_pbs_epic_slides.pdf"/>
+    <hyperlink ref="J9" r:id="rId29" display="https://neil3d.github.io/unreal/pbr-ue4.html"/>
+    <hyperlink ref="K9" r:id="rId30" display="assets\slides\s2013_pbs_epic_notes_v2.pdf"/>
+    <hyperlink ref="C15" r:id="rId31"/>
+    <hyperlink ref="G15" r:id="rId32" display="assets\thumb\cook-brdf.png"/>
+    <hyperlink ref="I15" r:id="rId33" display="assets\paper\p7-cook.pdf"/>
+    <hyperlink ref="C10" r:id="rId34"/>
+    <hyperlink ref="G10" r:id="rId35" display="assets\thumb\intro_dxr_sig2018.png"/>
+    <hyperlink ref="H10" r:id="rId36"/>
+    <hyperlink ref="I10" r:id="rId37" display="assets\slides\s2018_IntroDXR_RaytracingShaders.pdf"/>
+    <hyperlink ref="J10" r:id="rId38" display="https://neil3d.github.io/3dengine/DXRPreview.html"/>
+    <hyperlink ref="K10" r:id="rId39"/>
+    <hyperlink ref="K12" r:id="rId40"/>
+    <hyperlink ref="J12" r:id="rId41" display="https://neil3d.github.io/3dengine/why-ecs.html"/>
+    <hyperlink ref="C8" r:id="rId42"/>
+    <hyperlink ref="G8" r:id="rId43" display="assets\thumb\disney_pbs_sig2012.png"/>
+    <hyperlink ref="I8" r:id="rId44" display="assets\slides\s2012_pbs_disney_brdf_slides_v2.pdf"/>
+    <hyperlink ref="K8" r:id="rId45" display="assets\slides\s2012_pbs_disney_brdf_notes_v3.pdf"/>
+    <hyperlink ref="G16" r:id="rId46"/>
+    <hyperlink ref="I16" r:id="rId47"/>
+    <hyperlink ref="I17" r:id="rId48"/>
+    <hyperlink ref="C18" r:id="rId49"/>
+    <hyperlink ref="I18" r:id="rId50"/>
+    <hyperlink ref="G17" r:id="rId51"/>
+    <hyperlink ref="G18" r:id="rId52"/>
+    <hyperlink ref="C6" r:id="rId53"/>
+    <hyperlink ref="G6" r:id="rId54"/>
+    <hyperlink ref="H6" r:id="rId55"/>
+    <hyperlink ref="I6" r:id="rId56"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId53"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId57"/>
   <tableParts count="1">
-    <tablePart r:id="rId54"/>
+    <tablePart r:id="rId58"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
post SIGGRAPH 2015 Next Gen API
</commit_message>
<xml_diff>
--- a/reading/readings.xlsx
+++ b/reading/readings.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="d">Sheet1!$L$17</definedName>
-    <definedName name="ha">Sheet1!$L$17</definedName>
+    <definedName name="d">Sheet1!$L$18</definedName>
+    <definedName name="ha">Sheet1!$L$18</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="185">
   <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -660,6 +660,39 @@
   </si>
   <si>
     <t>《Effective C++》看过吧，那你必须看看 这个演讲，犀利，洗脑！Scott Meyers 依然给力！</t>
+  </si>
+  <si>
+    <t>Chris Wyman, Tim Foley…</t>
+  </si>
+  <si>
+    <t>http://nextgenapis.realtimerendering.com</t>
+  </si>
+  <si>
+    <t>2015年8月</t>
+  </si>
+  <si>
+    <t>SIGGRAPH 2015</t>
+  </si>
+  <si>
+    <t>3D API</t>
+  </si>
+  <si>
+    <t>assets/thumb/s2015_NextGenAPI.png</t>
+  </si>
+  <si>
+    <t>https://youtu.be/DXYROo5YAdI</t>
+  </si>
+  <si>
+    <t>assets/slides/s2015_NextGenAPI.zip</t>
+  </si>
+  <si>
+    <t>/3dengine/gl-brief-history.html</t>
+  </si>
+  <si>
+    <t>Vulkan，DX12都来一个简单介绍（也谈到Metal），并比较它们的异同。</t>
+  </si>
+  <si>
+    <t>An Overview of Next-Generation Graphics APIs</t>
   </si>
 </sst>
 </file>
@@ -830,7 +863,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L18" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L19" totalsRowShown="0" headerRowDxfId="10">
   <tableColumns count="12">
     <tableColumn id="1" name="title" dataDxfId="9"/>
     <tableColumn id="8" name="author" dataDxfId="8"/>
@@ -1112,11 +1145,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1245,581 +1278,621 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>174</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>15</v>
+        <v>175</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>48</v>
+        <v>176</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>177</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
+        <v>178</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>139</v>
+        <v>179</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>12</v>
+        <v>180</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>140</v>
+        <v>181</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>110</v>
+        <v>182</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="1" t="s">
-        <v>81</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>24</v>
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>110</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="1" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>166</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>167</v>
+        <v>24</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>169</v>
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>171</v>
+        <v>22</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="J6" s="9"/>
+        <v>142</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>110</v>
+      </c>
       <c r="K6" s="9"/>
       <c r="L6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="1" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>78</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="H8" s="7"/>
+        <v>143</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="I8" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="J8" s="9"/>
+        <v>144</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>111</v>
+      </c>
       <c r="K8" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D10" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>85</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I10" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J10" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K10" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="75" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:12" ht="75" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C11" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D11" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>98</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H11" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I11" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J11" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K11" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D12" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G12" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H12" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I12" s="9" t="s">
         <v>155</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="K11" s="9"/>
-      <c r="L11" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="K12" s="9"/>
+      <c r="L12" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="K13" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D14" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G14" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I14" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="J14" s="9" t="s">
         <v>111</v>
-      </c>
-      <c r="K13" s="9"/>
-      <c r="L13" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>110</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>119</v>
+        <v>41</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K15" s="9"/>
       <c r="L15" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="K16" s="9"/>
+      <c r="L16" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D17" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>118</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E17" t="s">
-        <v>130</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>131</v>
+        <v>164</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="E18" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G18" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I19" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>136</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1"/>
-    <hyperlink ref="C4" r:id="rId2"/>
-    <hyperlink ref="C14" r:id="rId3"/>
-    <hyperlink ref="H5" r:id="rId4"/>
-    <hyperlink ref="I4" r:id="rId5" display="assets\slides\oop_is_dead_long_live_dataoriented_design__stoyan_nikolov__cppcon_2018.pdf"/>
-    <hyperlink ref="I14" r:id="rId6" display="assets\slides\Introduction_to_Data-Oriented_Design_2014DICE.pdf"/>
-    <hyperlink ref="I5" r:id="rId7" display="assets\slides\Data-Oriented Design and C++ - Mike Acton - CppCon 2014.pptx"/>
-    <hyperlink ref="I11" r:id="rId8" display="assets\slides\GDC17-framegraph.pptx"/>
-    <hyperlink ref="C11" r:id="rId9"/>
-    <hyperlink ref="G4" r:id="rId10" display="assets\thumb\oop_is_dead_cppcon2018.png"/>
-    <hyperlink ref="G14" r:id="rId11" display="assets\thumb\dod_dice.png"/>
-    <hyperlink ref="G5" r:id="rId12" display="assets\thumb\dod_cppcon2014.png"/>
-    <hyperlink ref="G11" r:id="rId13" display="assets\thumb\framegraph_gdc2018.png"/>
-    <hyperlink ref="C13" r:id="rId14"/>
-    <hyperlink ref="G13" r:id="rId15" display="assets\thumb\the_rendering_equation.png"/>
-    <hyperlink ref="I13" r:id="rId16" display="assets\paper\p143-kajiya.pdf"/>
-    <hyperlink ref="H12" r:id="rId17"/>
-    <hyperlink ref="C12" r:id="rId18"/>
-    <hyperlink ref="G12" r:id="rId19" display="assets\thumb\overwatch_ecs_gdc2017.png"/>
-    <hyperlink ref="J4" r:id="rId20" display="https://neil3d.github.io/3dengine/why-ecs.html"/>
-    <hyperlink ref="C7" r:id="rId21"/>
-    <hyperlink ref="G7" r:id="rId22" display="assets\thumb\pbr_background_sig2013.png"/>
-    <hyperlink ref="H7" r:id="rId23"/>
-    <hyperlink ref="I7" r:id="rId24" display="assets\slides\s2013_pbs_physics_math_slides.pdf"/>
-    <hyperlink ref="K7" r:id="rId25" display="assets\slides\s2013_pbs_physics_math_notes.pdf"/>
-    <hyperlink ref="C9" r:id="rId26"/>
-    <hyperlink ref="G9" r:id="rId27" display="assets\thumb\ue4_pbr_sig2013.png"/>
-    <hyperlink ref="I9" r:id="rId28" display="assets\slides\s2013_pbs_epic_slides.pdf"/>
-    <hyperlink ref="J9" r:id="rId29" display="https://neil3d.github.io/unreal/pbr-ue4.html"/>
-    <hyperlink ref="K9" r:id="rId30" display="assets\slides\s2013_pbs_epic_notes_v2.pdf"/>
-    <hyperlink ref="C15" r:id="rId31"/>
-    <hyperlink ref="G15" r:id="rId32" display="assets\thumb\cook-brdf.png"/>
-    <hyperlink ref="I15" r:id="rId33" display="assets\paper\p7-cook.pdf"/>
-    <hyperlink ref="C10" r:id="rId34"/>
-    <hyperlink ref="G10" r:id="rId35" display="assets\thumb\intro_dxr_sig2018.png"/>
-    <hyperlink ref="H10" r:id="rId36"/>
-    <hyperlink ref="I10" r:id="rId37" display="assets\slides\s2018_IntroDXR_RaytracingShaders.pdf"/>
-    <hyperlink ref="J10" r:id="rId38" display="https://neil3d.github.io/3dengine/DXRPreview.html"/>
-    <hyperlink ref="K10" r:id="rId39"/>
-    <hyperlink ref="K12" r:id="rId40"/>
-    <hyperlink ref="J12" r:id="rId41" display="https://neil3d.github.io/3dengine/why-ecs.html"/>
-    <hyperlink ref="C8" r:id="rId42"/>
-    <hyperlink ref="G8" r:id="rId43" display="assets\thumb\disney_pbs_sig2012.png"/>
-    <hyperlink ref="I8" r:id="rId44" display="assets\slides\s2012_pbs_disney_brdf_slides_v2.pdf"/>
-    <hyperlink ref="K8" r:id="rId45" display="assets\slides\s2012_pbs_disney_brdf_notes_v3.pdf"/>
-    <hyperlink ref="G16" r:id="rId46"/>
-    <hyperlink ref="I16" r:id="rId47"/>
-    <hyperlink ref="I17" r:id="rId48"/>
-    <hyperlink ref="C18" r:id="rId49"/>
-    <hyperlink ref="I18" r:id="rId50"/>
-    <hyperlink ref="G17" r:id="rId51"/>
-    <hyperlink ref="G18" r:id="rId52"/>
-    <hyperlink ref="C6" r:id="rId53"/>
-    <hyperlink ref="G6" r:id="rId54"/>
-    <hyperlink ref="H6" r:id="rId55"/>
-    <hyperlink ref="I6" r:id="rId56"/>
+    <hyperlink ref="H5" r:id="rId1"/>
+    <hyperlink ref="C5" r:id="rId2"/>
+    <hyperlink ref="C15" r:id="rId3"/>
+    <hyperlink ref="H6" r:id="rId4"/>
+    <hyperlink ref="I5" r:id="rId5" display="assets\slides\oop_is_dead_long_live_dataoriented_design__stoyan_nikolov__cppcon_2018.pdf"/>
+    <hyperlink ref="I15" r:id="rId6" display="assets\slides\Introduction_to_Data-Oriented_Design_2014DICE.pdf"/>
+    <hyperlink ref="I6" r:id="rId7" display="assets\slides\Data-Oriented Design and C++ - Mike Acton - CppCon 2014.pptx"/>
+    <hyperlink ref="I12" r:id="rId8" display="assets\slides\GDC17-framegraph.pptx"/>
+    <hyperlink ref="C12" r:id="rId9"/>
+    <hyperlink ref="G5" r:id="rId10" display="assets\thumb\oop_is_dead_cppcon2018.png"/>
+    <hyperlink ref="G15" r:id="rId11" display="assets\thumb\dod_dice.png"/>
+    <hyperlink ref="G6" r:id="rId12" display="assets\thumb\dod_cppcon2014.png"/>
+    <hyperlink ref="G12" r:id="rId13" display="assets\thumb\framegraph_gdc2018.png"/>
+    <hyperlink ref="C14" r:id="rId14"/>
+    <hyperlink ref="G14" r:id="rId15" display="assets\thumb\the_rendering_equation.png"/>
+    <hyperlink ref="I14" r:id="rId16" display="assets\paper\p143-kajiya.pdf"/>
+    <hyperlink ref="H13" r:id="rId17"/>
+    <hyperlink ref="C13" r:id="rId18"/>
+    <hyperlink ref="G13" r:id="rId19" display="assets\thumb\overwatch_ecs_gdc2017.png"/>
+    <hyperlink ref="J5" r:id="rId20" display="https://neil3d.github.io/3dengine/why-ecs.html"/>
+    <hyperlink ref="C8" r:id="rId21"/>
+    <hyperlink ref="G8" r:id="rId22" display="assets\thumb\pbr_background_sig2013.png"/>
+    <hyperlink ref="H8" r:id="rId23"/>
+    <hyperlink ref="I8" r:id="rId24" display="assets\slides\s2013_pbs_physics_math_slides.pdf"/>
+    <hyperlink ref="K8" r:id="rId25" display="assets\slides\s2013_pbs_physics_math_notes.pdf"/>
+    <hyperlink ref="C10" r:id="rId26"/>
+    <hyperlink ref="G10" r:id="rId27" display="assets\thumb\ue4_pbr_sig2013.png"/>
+    <hyperlink ref="I10" r:id="rId28" display="assets\slides\s2013_pbs_epic_slides.pdf"/>
+    <hyperlink ref="J10" r:id="rId29" display="https://neil3d.github.io/unreal/pbr-ue4.html"/>
+    <hyperlink ref="K10" r:id="rId30" display="assets\slides\s2013_pbs_epic_notes_v2.pdf"/>
+    <hyperlink ref="C16" r:id="rId31"/>
+    <hyperlink ref="G16" r:id="rId32" display="assets\thumb\cook-brdf.png"/>
+    <hyperlink ref="I16" r:id="rId33" display="assets\paper\p7-cook.pdf"/>
+    <hyperlink ref="C11" r:id="rId34"/>
+    <hyperlink ref="G11" r:id="rId35" display="assets\thumb\intro_dxr_sig2018.png"/>
+    <hyperlink ref="H11" r:id="rId36"/>
+    <hyperlink ref="I11" r:id="rId37" display="assets\slides\s2018_IntroDXR_RaytracingShaders.pdf"/>
+    <hyperlink ref="J11" r:id="rId38" display="https://neil3d.github.io/3dengine/DXRPreview.html"/>
+    <hyperlink ref="K11" r:id="rId39"/>
+    <hyperlink ref="K13" r:id="rId40"/>
+    <hyperlink ref="J13" r:id="rId41" display="https://neil3d.github.io/3dengine/why-ecs.html"/>
+    <hyperlink ref="C9" r:id="rId42"/>
+    <hyperlink ref="G9" r:id="rId43" display="assets\thumb\disney_pbs_sig2012.png"/>
+    <hyperlink ref="I9" r:id="rId44" display="assets\slides\s2012_pbs_disney_brdf_slides_v2.pdf"/>
+    <hyperlink ref="K9" r:id="rId45" display="assets\slides\s2012_pbs_disney_brdf_notes_v3.pdf"/>
+    <hyperlink ref="G17" r:id="rId46"/>
+    <hyperlink ref="I17" r:id="rId47"/>
+    <hyperlink ref="I18" r:id="rId48"/>
+    <hyperlink ref="C19" r:id="rId49"/>
+    <hyperlink ref="I19" r:id="rId50"/>
+    <hyperlink ref="G18" r:id="rId51"/>
+    <hyperlink ref="G19" r:id="rId52"/>
+    <hyperlink ref="C7" r:id="rId53"/>
+    <hyperlink ref="G7" r:id="rId54"/>
+    <hyperlink ref="H7" r:id="rId55"/>
+    <hyperlink ref="I7" r:id="rId56"/>
+    <hyperlink ref="C4" r:id="rId57"/>
+    <hyperlink ref="G4" r:id="rId58"/>
+    <hyperlink ref="H4" r:id="rId59"/>
+    <hyperlink ref="I4" r:id="rId60"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId57"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId61"/>
   <tableParts count="1">
-    <tablePart r:id="rId58"/>
+    <tablePart r:id="rId62"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add BRDF lecture thumb
</commit_message>
<xml_diff>
--- a/reading/readings.xlsx
+++ b/reading/readings.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="194">
   <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -717,6 +717,9 @@
   </si>
   <si>
     <t>一个很好的BRDF的讲义</t>
+  </si>
+  <si>
+    <t>assets/thumb/brdf-lecture.png</t>
   </si>
 </sst>
 </file>
@@ -1173,7 +1176,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
+      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1779,7 +1782,7 @@
         <v>120</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>161</v>
+        <v>193</v>
       </c>
       <c r="I17" s="9" t="s">
         <v>191</v>
@@ -1943,8 +1946,8 @@
     <hyperlink ref="G4" r:id="rId58"/>
     <hyperlink ref="H4" r:id="rId59"/>
     <hyperlink ref="I4" r:id="rId60"/>
-    <hyperlink ref="G17" r:id="rId61" display="assets\thumb\cook-brdf.png"/>
-    <hyperlink ref="I17" r:id="rId62"/>
+    <hyperlink ref="I17" r:id="rId61"/>
+    <hyperlink ref="G17" r:id="rId62"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId63"/>

</xml_diff>

<commit_message>
sort readings by date
</commit_message>
<xml_diff>
--- a/reading/readings.xlsx
+++ b/reading/readings.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="d">Sheet1!$L$19</definedName>
-    <definedName name="ha">Sheet1!$L$19</definedName>
+    <definedName name="d">Sheet1!$L$17</definedName>
+    <definedName name="ha">Sheet1!$L$17</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="175">
   <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,14 +56,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>author</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -72,10 +64,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>publisher</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -136,46 +124,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>作者</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>主页</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>发布日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>发布者</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>标签</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>缩略图</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>视频</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>文档</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>简介</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -208,10 +156,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DIC工作室对于面向数据的设计的一个分享。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -224,10 +168,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2018年10月</t>
   </si>
   <si>
@@ -300,23 +240,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>相关博文</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>notes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>课程笔记</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -726,7 +650,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -736,15 +660,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
@@ -787,9 +702,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -797,27 +712,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -890,7 +796,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L20" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L18" totalsRowShown="0" headerRowDxfId="10">
+  <sortState ref="A2:L18">
+    <sortCondition descending="1" ref="D2:D18"/>
+  </sortState>
   <tableColumns count="12">
     <tableColumn id="1" name="title" dataDxfId="9"/>
     <tableColumn id="8" name="author" dataDxfId="8"/>
@@ -1172,17 +1081,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="23.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="12" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="9" customWidth="1"/>
     <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.33203125" style="1" customWidth="1"/>
@@ -1196,16 +1105,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1</v>
@@ -1217,737 +1126,661 @@
         <v>3</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="I3" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>6</v>
+      <c r="F5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="E4" t="s">
-        <v>177</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="K5" s="9"/>
-      <c r="L5" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>50</v>
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>157</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>158</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="K6" s="9"/>
+        <v>159</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="K6" s="7"/>
       <c r="L6" s="1" t="s">
-        <v>45</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
+      <c r="G7" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K7" s="7"/>
       <c r="L7" s="1" t="s">
-        <v>173</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>73</v>
+        <v>147</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" t="s">
-        <v>77</v>
+        <v>146</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>145</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
       <c r="L8" s="1" t="s">
-        <v>80</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>109</v>
+        <v>63</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9" t="s">
-        <v>148</v>
+        <v>67</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>84</v>
+        <v>55</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="E10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="L10" s="1" t="s">
+      <c r="C11" s="7" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="75" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>97</v>
+      <c r="D11" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="E11" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>101</v>
+        <v>59</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7" t="s">
+        <v>129</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>51</v>
+        <v>14</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="K12" s="9"/>
+        <v>28</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" s="7"/>
       <c r="L12" s="1" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>57</v>
+        <v>167</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>63</v>
+        <v>168</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>171</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>103</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
       <c r="L13" s="1" t="s">
-        <v>114</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>54</v>
+        <v>37</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="K14" s="9"/>
+        <v>101</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K14" s="7"/>
       <c r="L14" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>49</v>
+        <v>70</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="K15" s="9"/>
+        <v>100</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K15" s="7"/>
       <c r="L15" s="1" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>88</v>
+        <v>145</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>91</v>
+        <v>105</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>107</v>
       </c>
       <c r="E16" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="K16" s="9"/>
+        <v>101</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="L16" s="1" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>186</v>
+        <v>144</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>189</v>
+        <v>96</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>98</v>
       </c>
       <c r="E17" t="s">
-        <v>190</v>
+        <v>99</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
+        <v>101</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>103</v>
+      </c>
       <c r="L17" s="1" t="s">
-        <v>192</v>
+        <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>163</v>
+        <v>112</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" t="s">
         <v>115</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="F18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I18" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="L18" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="E18" t="s">
-        <v>118</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E19" t="s">
-        <v>130</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E20" t="s">
-        <v>134</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H5" r:id="rId1"/>
-    <hyperlink ref="C5" r:id="rId2"/>
-    <hyperlink ref="C15" r:id="rId3"/>
-    <hyperlink ref="H6" r:id="rId4"/>
-    <hyperlink ref="I5" r:id="rId5" display="assets\slides\oop_is_dead_long_live_dataoriented_design__stoyan_nikolov__cppcon_2018.pdf"/>
-    <hyperlink ref="I15" r:id="rId6" display="assets\slides\Introduction_to_Data-Oriented_Design_2014DICE.pdf"/>
-    <hyperlink ref="I6" r:id="rId7" display="assets\slides\Data-Oriented Design and C++ - Mike Acton - CppCon 2014.pptx"/>
-    <hyperlink ref="I12" r:id="rId8" display="assets\slides\GDC17-framegraph.pptx"/>
-    <hyperlink ref="C12" r:id="rId9"/>
-    <hyperlink ref="G5" r:id="rId10" display="assets\thumb\oop_is_dead_cppcon2018.png"/>
-    <hyperlink ref="G15" r:id="rId11" display="assets\thumb\dod_dice.png"/>
-    <hyperlink ref="G6" r:id="rId12" display="assets\thumb\dod_cppcon2014.png"/>
-    <hyperlink ref="G12" r:id="rId13" display="assets\thumb\framegraph_gdc2018.png"/>
+    <hyperlink ref="H3" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C12" r:id="rId3"/>
+    <hyperlink ref="H7" r:id="rId4"/>
+    <hyperlink ref="I3" r:id="rId5" display="assets\slides\oop_is_dead_long_live_dataoriented_design__stoyan_nikolov__cppcon_2018.pdf"/>
+    <hyperlink ref="I12" r:id="rId6" display="assets\slides\Introduction_to_Data-Oriented_Design_2014DICE.pdf"/>
+    <hyperlink ref="I7" r:id="rId7" display="assets\slides\Data-Oriented Design and C++ - Mike Acton - CppCon 2014.pptx"/>
+    <hyperlink ref="I4" r:id="rId8" display="assets\slides\GDC17-framegraph.pptx"/>
+    <hyperlink ref="C4" r:id="rId9"/>
+    <hyperlink ref="G3" r:id="rId10" display="assets\thumb\oop_is_dead_cppcon2018.png"/>
+    <hyperlink ref="G12" r:id="rId11" display="assets\thumb\dod_dice.png"/>
+    <hyperlink ref="G7" r:id="rId12" display="assets\thumb\dod_cppcon2014.png"/>
+    <hyperlink ref="G4" r:id="rId13" display="assets\thumb\framegraph_gdc2018.png"/>
     <hyperlink ref="C14" r:id="rId14"/>
     <hyperlink ref="G14" r:id="rId15" display="assets\thumb\the_rendering_equation.png"/>
     <hyperlink ref="I14" r:id="rId16" display="assets\paper\p143-kajiya.pdf"/>
-    <hyperlink ref="H13" r:id="rId17"/>
-    <hyperlink ref="C13" r:id="rId18"/>
-    <hyperlink ref="G13" r:id="rId19" display="assets\thumb\overwatch_ecs_gdc2017.png"/>
-    <hyperlink ref="J5" r:id="rId20" display="https://neil3d.github.io/3dengine/why-ecs.html"/>
-    <hyperlink ref="C8" r:id="rId21"/>
-    <hyperlink ref="G8" r:id="rId22" display="assets\thumb\pbr_background_sig2013.png"/>
-    <hyperlink ref="H8" r:id="rId23"/>
-    <hyperlink ref="I8" r:id="rId24" display="assets\slides\s2013_pbs_physics_math_slides.pdf"/>
-    <hyperlink ref="K8" r:id="rId25" display="assets\slides\s2013_pbs_physics_math_notes.pdf"/>
-    <hyperlink ref="C10" r:id="rId26"/>
-    <hyperlink ref="G10" r:id="rId27" display="assets\thumb\ue4_pbr_sig2013.png"/>
-    <hyperlink ref="I10" r:id="rId28" display="assets\slides\s2013_pbs_epic_slides.pdf"/>
-    <hyperlink ref="J10" r:id="rId29" display="https://neil3d.github.io/unreal/pbr-ue4.html"/>
-    <hyperlink ref="K10" r:id="rId30" display="assets\slides\s2013_pbs_epic_notes_v2.pdf"/>
-    <hyperlink ref="C16" r:id="rId31"/>
-    <hyperlink ref="G16" r:id="rId32" display="assets\thumb\cook-brdf.png"/>
-    <hyperlink ref="I16" r:id="rId33" display="assets\paper\p7-cook.pdf"/>
-    <hyperlink ref="C11" r:id="rId34"/>
-    <hyperlink ref="G11" r:id="rId35" display="assets\thumb\intro_dxr_sig2018.png"/>
-    <hyperlink ref="H11" r:id="rId36"/>
-    <hyperlink ref="I11" r:id="rId37" display="assets\slides\s2018_IntroDXR_RaytracingShaders.pdf"/>
-    <hyperlink ref="J11" r:id="rId38" display="https://neil3d.github.io/3dengine/DXRPreview.html"/>
-    <hyperlink ref="K11" r:id="rId39"/>
-    <hyperlink ref="K13" r:id="rId40"/>
-    <hyperlink ref="J13" r:id="rId41" display="https://neil3d.github.io/3dengine/why-ecs.html"/>
-    <hyperlink ref="C9" r:id="rId42"/>
-    <hyperlink ref="G9" r:id="rId43" display="assets\thumb\disney_pbs_sig2012.png"/>
-    <hyperlink ref="I9" r:id="rId44" display="assets\slides\s2012_pbs_disney_brdf_slides_v2.pdf"/>
-    <hyperlink ref="K9" r:id="rId45" display="assets\slides\s2012_pbs_disney_brdf_notes_v3.pdf"/>
-    <hyperlink ref="G18" r:id="rId46"/>
-    <hyperlink ref="I18" r:id="rId47"/>
-    <hyperlink ref="I19" r:id="rId48"/>
-    <hyperlink ref="C20" r:id="rId49"/>
-    <hyperlink ref="I20" r:id="rId50"/>
-    <hyperlink ref="G19" r:id="rId51"/>
-    <hyperlink ref="G20" r:id="rId52"/>
-    <hyperlink ref="C7" r:id="rId53"/>
-    <hyperlink ref="G7" r:id="rId54"/>
-    <hyperlink ref="H7" r:id="rId55"/>
-    <hyperlink ref="I7" r:id="rId56"/>
-    <hyperlink ref="C4" r:id="rId57"/>
-    <hyperlink ref="G4" r:id="rId58"/>
-    <hyperlink ref="H4" r:id="rId59"/>
-    <hyperlink ref="I4" r:id="rId60"/>
-    <hyperlink ref="I17" r:id="rId61"/>
-    <hyperlink ref="G17" r:id="rId62"/>
+    <hyperlink ref="H5" r:id="rId17"/>
+    <hyperlink ref="C5" r:id="rId18"/>
+    <hyperlink ref="G5" r:id="rId19" display="assets\thumb\overwatch_ecs_gdc2017.png"/>
+    <hyperlink ref="J3" r:id="rId20" display="https://neil3d.github.io/3dengine/why-ecs.html"/>
+    <hyperlink ref="C10" r:id="rId21"/>
+    <hyperlink ref="G10" r:id="rId22" display="assets\thumb\pbr_background_sig2013.png"/>
+    <hyperlink ref="H10" r:id="rId23"/>
+    <hyperlink ref="I10" r:id="rId24" display="assets\slides\s2013_pbs_physics_math_slides.pdf"/>
+    <hyperlink ref="K10" r:id="rId25" display="assets\slides\s2013_pbs_physics_math_notes.pdf"/>
+    <hyperlink ref="C9" r:id="rId26"/>
+    <hyperlink ref="G9" r:id="rId27" display="assets\thumb\ue4_pbr_sig2013.png"/>
+    <hyperlink ref="I9" r:id="rId28" display="assets\slides\s2013_pbs_epic_slides.pdf"/>
+    <hyperlink ref="J9" r:id="rId29" display="https://neil3d.github.io/unreal/pbr-ue4.html"/>
+    <hyperlink ref="K9" r:id="rId30" display="assets\slides\s2013_pbs_epic_notes_v2.pdf"/>
+    <hyperlink ref="C15" r:id="rId31"/>
+    <hyperlink ref="G15" r:id="rId32" display="assets\thumb\cook-brdf.png"/>
+    <hyperlink ref="I15" r:id="rId33" display="assets\paper\p7-cook.pdf"/>
+    <hyperlink ref="C2" r:id="rId34"/>
+    <hyperlink ref="G2" r:id="rId35" display="assets\thumb\intro_dxr_sig2018.png"/>
+    <hyperlink ref="H2" r:id="rId36"/>
+    <hyperlink ref="I2" r:id="rId37" display="assets\slides\s2018_IntroDXR_RaytracingShaders.pdf"/>
+    <hyperlink ref="J2" r:id="rId38" display="https://neil3d.github.io/3dengine/DXRPreview.html"/>
+    <hyperlink ref="K2" r:id="rId39"/>
+    <hyperlink ref="K5" r:id="rId40"/>
+    <hyperlink ref="J5" r:id="rId41" display="https://neil3d.github.io/3dengine/why-ecs.html"/>
+    <hyperlink ref="C11" r:id="rId42"/>
+    <hyperlink ref="G11" r:id="rId43" display="assets\thumb\disney_pbs_sig2012.png"/>
+    <hyperlink ref="I11" r:id="rId44" display="assets\slides\s2012_pbs_disney_brdf_slides_v2.pdf"/>
+    <hyperlink ref="K11" r:id="rId45" display="assets\slides\s2012_pbs_disney_brdf_notes_v3.pdf"/>
+    <hyperlink ref="G17" r:id="rId46"/>
+    <hyperlink ref="I17" r:id="rId47"/>
+    <hyperlink ref="I16" r:id="rId48"/>
+    <hyperlink ref="C18" r:id="rId49"/>
+    <hyperlink ref="I18" r:id="rId50"/>
+    <hyperlink ref="G16" r:id="rId51"/>
+    <hyperlink ref="G18" r:id="rId52"/>
+    <hyperlink ref="C8" r:id="rId53"/>
+    <hyperlink ref="G8" r:id="rId54"/>
+    <hyperlink ref="H8" r:id="rId55"/>
+    <hyperlink ref="I8" r:id="rId56"/>
+    <hyperlink ref="C6" r:id="rId57"/>
+    <hyperlink ref="G6" r:id="rId58"/>
+    <hyperlink ref="H6" r:id="rId59"/>
+    <hyperlink ref="I6" r:id="rId60"/>
+    <hyperlink ref="I13" r:id="rId61"/>
+    <hyperlink ref="G13" r:id="rId62"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId63"/>

</xml_diff>

<commit_message>
add gdc 2002 components talk
</commit_message>
<xml_diff>
--- a/reading/readings.xlsx
+++ b/reading/readings.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="183">
   <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -644,6 +644,31 @@
   </si>
   <si>
     <t>assets/thumb/brdf-lecture.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A Data-Driven
+Game Object System</t>
+  </si>
+  <si>
+    <t>Scott Bilas</t>
+  </si>
+  <si>
+    <t>2002年3月</t>
+  </si>
+  <si>
+    <t>GDC 2002</t>
+  </si>
+  <si>
+    <t>引擎架构</t>
+  </si>
+  <si>
+    <t>assets/thumb/gdc02-components.png</t>
+  </si>
+  <si>
+    <t>assets/slides/data-driven-game-object-system.pdf</t>
+  </si>
+  <si>
+    <t>我看到的最早的发表的谈论Component组件对象模型的演讲，是由《地牢围攻》开发者在GDC 2002做的分享。</t>
   </si>
 </sst>
 </file>
@@ -796,9 +821,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L18" totalsRowShown="0" headerRowDxfId="10">
-  <sortState ref="A2:L18">
-    <sortCondition descending="1" ref="D2:D18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L19" totalsRowShown="0" headerRowDxfId="10">
+  <sortState ref="A2:L19">
+    <sortCondition descending="1" ref="D2:D19"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" name="title" dataDxfId="9"/>
@@ -1081,11 +1106,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1560,159 +1585,185 @@
         <v>173</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>175</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>38</v>
+        <v>176</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>39</v>
+        <v>177</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>178</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>101</v>
+        <v>179</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>138</v>
+        <v>180</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K14" s="7"/>
+        <v>181</v>
+      </c>
       <c r="L14" s="1" t="s">
-        <v>41</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J15" s="7" t="s">
         <v>92</v>
       </c>
       <c r="K15" s="7"/>
       <c r="L15" s="1" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K16" s="7"/>
+      <c r="L16" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D17" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>111</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="E17" t="s">
-        <v>99</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>101</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>103</v>
+        <v>108</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>114</v>
+        <v>96</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>98</v>
       </c>
       <c r="E18" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>101</v>
       </c>
       <c r="G18" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" t="s">
+        <v>115</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G19" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I19" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1732,9 +1783,9 @@
     <hyperlink ref="G12" r:id="rId11" display="assets\thumb\dod_dice.png"/>
     <hyperlink ref="G7" r:id="rId12" display="assets\thumb\dod_cppcon2014.png"/>
     <hyperlink ref="G4" r:id="rId13" display="assets\thumb\framegraph_gdc2018.png"/>
-    <hyperlink ref="C14" r:id="rId14"/>
-    <hyperlink ref="G14" r:id="rId15" display="assets\thumb\the_rendering_equation.png"/>
-    <hyperlink ref="I14" r:id="rId16" display="assets\paper\p143-kajiya.pdf"/>
+    <hyperlink ref="C15" r:id="rId14"/>
+    <hyperlink ref="G15" r:id="rId15" display="assets\thumb\the_rendering_equation.png"/>
+    <hyperlink ref="I15" r:id="rId16" display="assets\paper\p143-kajiya.pdf"/>
     <hyperlink ref="H5" r:id="rId17"/>
     <hyperlink ref="C5" r:id="rId18"/>
     <hyperlink ref="G5" r:id="rId19" display="assets\thumb\overwatch_ecs_gdc2017.png"/>
@@ -1749,9 +1800,9 @@
     <hyperlink ref="I9" r:id="rId28" display="assets\slides\s2013_pbs_epic_slides.pdf"/>
     <hyperlink ref="J9" r:id="rId29" display="https://neil3d.github.io/unreal/pbr-ue4.html"/>
     <hyperlink ref="K9" r:id="rId30" display="assets\slides\s2013_pbs_epic_notes_v2.pdf"/>
-    <hyperlink ref="C15" r:id="rId31"/>
-    <hyperlink ref="G15" r:id="rId32" display="assets\thumb\cook-brdf.png"/>
-    <hyperlink ref="I15" r:id="rId33" display="assets\paper\p7-cook.pdf"/>
+    <hyperlink ref="C16" r:id="rId31"/>
+    <hyperlink ref="G16" r:id="rId32" display="assets\thumb\cook-brdf.png"/>
+    <hyperlink ref="I16" r:id="rId33" display="assets\paper\p7-cook.pdf"/>
     <hyperlink ref="C2" r:id="rId34"/>
     <hyperlink ref="G2" r:id="rId35" display="assets\thumb\intro_dxr_sig2018.png"/>
     <hyperlink ref="H2" r:id="rId36"/>
@@ -1764,13 +1815,13 @@
     <hyperlink ref="G11" r:id="rId43" display="assets\thumb\disney_pbs_sig2012.png"/>
     <hyperlink ref="I11" r:id="rId44" display="assets\slides\s2012_pbs_disney_brdf_slides_v2.pdf"/>
     <hyperlink ref="K11" r:id="rId45" display="assets\slides\s2012_pbs_disney_brdf_notes_v3.pdf"/>
-    <hyperlink ref="G17" r:id="rId46"/>
-    <hyperlink ref="I17" r:id="rId47"/>
-    <hyperlink ref="I16" r:id="rId48"/>
-    <hyperlink ref="C18" r:id="rId49"/>
-    <hyperlink ref="I18" r:id="rId50"/>
-    <hyperlink ref="G16" r:id="rId51"/>
-    <hyperlink ref="G18" r:id="rId52"/>
+    <hyperlink ref="G18" r:id="rId46"/>
+    <hyperlink ref="I18" r:id="rId47"/>
+    <hyperlink ref="I17" r:id="rId48"/>
+    <hyperlink ref="C19" r:id="rId49"/>
+    <hyperlink ref="I19" r:id="rId50"/>
+    <hyperlink ref="G17" r:id="rId51"/>
+    <hyperlink ref="G19" r:id="rId52"/>
     <hyperlink ref="C8" r:id="rId53"/>
     <hyperlink ref="G8" r:id="rId54"/>
     <hyperlink ref="H8" r:id="rId55"/>
@@ -1781,11 +1832,13 @@
     <hyperlink ref="I6" r:id="rId60"/>
     <hyperlink ref="I13" r:id="rId61"/>
     <hyperlink ref="G13" r:id="rId62"/>
+    <hyperlink ref="G14" r:id="rId63"/>
+    <hyperlink ref="I14" r:id="rId64"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId63"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId65"/>
   <tableParts count="1">
-    <tablePart r:id="rId64"/>
+    <tablePart r:id="rId66"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add gdc2014 designer programmer interaction talk
</commit_message>
<xml_diff>
--- a/reading/readings.xlsx
+++ b/reading/readings.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="192">
   <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -669,6 +669,33 @@
   </si>
   <si>
     <t>我看到的最早的发表的谈论Component组件对象模型的演讲，是由《地牢围攻》开发者在GDC 2002做的分享。</t>
+  </si>
+  <si>
+    <t>Designers Are from Saturn, Programmers Are from Uranus</t>
+  </si>
+  <si>
+    <t>2014年3月</t>
+  </si>
+  <si>
+    <t>GDC 2014</t>
+  </si>
+  <si>
+    <t>游戏开发</t>
+  </si>
+  <si>
+    <t>assets/thumb/gdc14-designer-programmer.png</t>
+  </si>
+  <si>
+    <t>assets/slides/Schwab_Brian_Designers_Are_From.pdf</t>
+  </si>
+  <si>
+    <t>很有趣的一个讲程序+策划工作配合的一个演讲。</t>
+  </si>
+  <si>
+    <t>Brian Schwab</t>
+  </si>
+  <si>
+    <t>https://youtu.be/6b-o_-Xb50E</t>
   </si>
 </sst>
 </file>
@@ -821,9 +848,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L19" totalsRowShown="0" headerRowDxfId="10">
-  <sortState ref="A2:L19">
-    <sortCondition descending="1" ref="D2:D19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L20" totalsRowShown="0" headerRowDxfId="10">
+  <sortState ref="A2:L20">
+    <sortCondition descending="1" ref="D2:D20"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" name="title" dataDxfId="9"/>
@@ -1106,11 +1133,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1380,390 +1407,419 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="E8" t="s">
+        <v>185</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D9" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I9" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="1" t="s">
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="1" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>56</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G11" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="7" t="s">
+      <c r="H12" s="5"/>
+      <c r="I12" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7" t="s">
+      <c r="J12" s="7"/>
+      <c r="K12" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D13" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G13" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I13" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J13" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="E13" t="s">
-        <v>171</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E14" t="s">
+        <v>171</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D15" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>178</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G15" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I15" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K15" s="7"/>
-      <c r="L15" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>92</v>
       </c>
       <c r="K16" s="7"/>
       <c r="L16" s="1" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K17" s="7"/>
+      <c r="L17" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>111</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="45" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="E18" t="s">
-        <v>99</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>101</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>103</v>
+        <v>108</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>114</v>
+        <v>96</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>98</v>
       </c>
       <c r="E19" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>101</v>
       </c>
       <c r="G19" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" t="s">
+        <v>115</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="I20" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1772,37 +1828,37 @@
   <hyperlinks>
     <hyperlink ref="H3" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C12" r:id="rId3"/>
+    <hyperlink ref="C13" r:id="rId3"/>
     <hyperlink ref="H7" r:id="rId4"/>
     <hyperlink ref="I3" r:id="rId5" display="assets\slides\oop_is_dead_long_live_dataoriented_design__stoyan_nikolov__cppcon_2018.pdf"/>
-    <hyperlink ref="I12" r:id="rId6" display="assets\slides\Introduction_to_Data-Oriented_Design_2014DICE.pdf"/>
+    <hyperlink ref="I13" r:id="rId6" display="assets\slides\Introduction_to_Data-Oriented_Design_2014DICE.pdf"/>
     <hyperlink ref="I7" r:id="rId7" display="assets\slides\Data-Oriented Design and C++ - Mike Acton - CppCon 2014.pptx"/>
     <hyperlink ref="I4" r:id="rId8" display="assets\slides\GDC17-framegraph.pptx"/>
     <hyperlink ref="C4" r:id="rId9"/>
     <hyperlink ref="G3" r:id="rId10" display="assets\thumb\oop_is_dead_cppcon2018.png"/>
-    <hyperlink ref="G12" r:id="rId11" display="assets\thumb\dod_dice.png"/>
+    <hyperlink ref="G13" r:id="rId11" display="assets\thumb\dod_dice.png"/>
     <hyperlink ref="G7" r:id="rId12" display="assets\thumb\dod_cppcon2014.png"/>
     <hyperlink ref="G4" r:id="rId13" display="assets\thumb\framegraph_gdc2018.png"/>
-    <hyperlink ref="C15" r:id="rId14"/>
-    <hyperlink ref="G15" r:id="rId15" display="assets\thumb\the_rendering_equation.png"/>
-    <hyperlink ref="I15" r:id="rId16" display="assets\paper\p143-kajiya.pdf"/>
+    <hyperlink ref="C16" r:id="rId14"/>
+    <hyperlink ref="G16" r:id="rId15" display="assets\thumb\the_rendering_equation.png"/>
+    <hyperlink ref="I16" r:id="rId16" display="assets\paper\p143-kajiya.pdf"/>
     <hyperlink ref="H5" r:id="rId17"/>
     <hyperlink ref="C5" r:id="rId18"/>
     <hyperlink ref="G5" r:id="rId19" display="assets\thumb\overwatch_ecs_gdc2017.png"/>
     <hyperlink ref="J3" r:id="rId20" display="https://neil3d.github.io/3dengine/why-ecs.html"/>
-    <hyperlink ref="C10" r:id="rId21"/>
-    <hyperlink ref="G10" r:id="rId22" display="assets\thumb\pbr_background_sig2013.png"/>
-    <hyperlink ref="H10" r:id="rId23"/>
-    <hyperlink ref="I10" r:id="rId24" display="assets\slides\s2013_pbs_physics_math_slides.pdf"/>
-    <hyperlink ref="K10" r:id="rId25" display="assets\slides\s2013_pbs_physics_math_notes.pdf"/>
-    <hyperlink ref="C9" r:id="rId26"/>
-    <hyperlink ref="G9" r:id="rId27" display="assets\thumb\ue4_pbr_sig2013.png"/>
-    <hyperlink ref="I9" r:id="rId28" display="assets\slides\s2013_pbs_epic_slides.pdf"/>
-    <hyperlink ref="J9" r:id="rId29" display="https://neil3d.github.io/unreal/pbr-ue4.html"/>
-    <hyperlink ref="K9" r:id="rId30" display="assets\slides\s2013_pbs_epic_notes_v2.pdf"/>
-    <hyperlink ref="C16" r:id="rId31"/>
-    <hyperlink ref="G16" r:id="rId32" display="assets\thumb\cook-brdf.png"/>
-    <hyperlink ref="I16" r:id="rId33" display="assets\paper\p7-cook.pdf"/>
+    <hyperlink ref="C11" r:id="rId21"/>
+    <hyperlink ref="G11" r:id="rId22" display="assets\thumb\pbr_background_sig2013.png"/>
+    <hyperlink ref="H11" r:id="rId23"/>
+    <hyperlink ref="I11" r:id="rId24" display="assets\slides\s2013_pbs_physics_math_slides.pdf"/>
+    <hyperlink ref="K11" r:id="rId25" display="assets\slides\s2013_pbs_physics_math_notes.pdf"/>
+    <hyperlink ref="C10" r:id="rId26"/>
+    <hyperlink ref="G10" r:id="rId27" display="assets\thumb\ue4_pbr_sig2013.png"/>
+    <hyperlink ref="I10" r:id="rId28" display="assets\slides\s2013_pbs_epic_slides.pdf"/>
+    <hyperlink ref="J10" r:id="rId29" display="https://neil3d.github.io/unreal/pbr-ue4.html"/>
+    <hyperlink ref="K10" r:id="rId30" display="assets\slides\s2013_pbs_epic_notes_v2.pdf"/>
+    <hyperlink ref="C17" r:id="rId31"/>
+    <hyperlink ref="G17" r:id="rId32" display="assets\thumb\cook-brdf.png"/>
+    <hyperlink ref="I17" r:id="rId33" display="assets\paper\p7-cook.pdf"/>
     <hyperlink ref="C2" r:id="rId34"/>
     <hyperlink ref="G2" r:id="rId35" display="assets\thumb\intro_dxr_sig2018.png"/>
     <hyperlink ref="H2" r:id="rId36"/>
@@ -1811,34 +1867,37 @@
     <hyperlink ref="K2" r:id="rId39"/>
     <hyperlink ref="K5" r:id="rId40"/>
     <hyperlink ref="J5" r:id="rId41" display="https://neil3d.github.io/3dengine/why-ecs.html"/>
-    <hyperlink ref="C11" r:id="rId42"/>
-    <hyperlink ref="G11" r:id="rId43" display="assets\thumb\disney_pbs_sig2012.png"/>
-    <hyperlink ref="I11" r:id="rId44" display="assets\slides\s2012_pbs_disney_brdf_slides_v2.pdf"/>
-    <hyperlink ref="K11" r:id="rId45" display="assets\slides\s2012_pbs_disney_brdf_notes_v3.pdf"/>
-    <hyperlink ref="G18" r:id="rId46"/>
-    <hyperlink ref="I18" r:id="rId47"/>
-    <hyperlink ref="I17" r:id="rId48"/>
-    <hyperlink ref="C19" r:id="rId49"/>
-    <hyperlink ref="I19" r:id="rId50"/>
-    <hyperlink ref="G17" r:id="rId51"/>
-    <hyperlink ref="G19" r:id="rId52"/>
-    <hyperlink ref="C8" r:id="rId53"/>
-    <hyperlink ref="G8" r:id="rId54"/>
-    <hyperlink ref="H8" r:id="rId55"/>
-    <hyperlink ref="I8" r:id="rId56"/>
+    <hyperlink ref="C12" r:id="rId42"/>
+    <hyperlink ref="G12" r:id="rId43" display="assets\thumb\disney_pbs_sig2012.png"/>
+    <hyperlink ref="I12" r:id="rId44" display="assets\slides\s2012_pbs_disney_brdf_slides_v2.pdf"/>
+    <hyperlink ref="K12" r:id="rId45" display="assets\slides\s2012_pbs_disney_brdf_notes_v3.pdf"/>
+    <hyperlink ref="G19" r:id="rId46"/>
+    <hyperlink ref="I19" r:id="rId47"/>
+    <hyperlink ref="I18" r:id="rId48"/>
+    <hyperlink ref="C20" r:id="rId49"/>
+    <hyperlink ref="I20" r:id="rId50"/>
+    <hyperlink ref="G18" r:id="rId51"/>
+    <hyperlink ref="G20" r:id="rId52"/>
+    <hyperlink ref="C9" r:id="rId53"/>
+    <hyperlink ref="G9" r:id="rId54"/>
+    <hyperlink ref="H9" r:id="rId55"/>
+    <hyperlink ref="I9" r:id="rId56"/>
     <hyperlink ref="C6" r:id="rId57"/>
     <hyperlink ref="G6" r:id="rId58"/>
     <hyperlink ref="H6" r:id="rId59"/>
     <hyperlink ref="I6" r:id="rId60"/>
-    <hyperlink ref="I13" r:id="rId61"/>
-    <hyperlink ref="G13" r:id="rId62"/>
-    <hyperlink ref="G14" r:id="rId63"/>
-    <hyperlink ref="I14" r:id="rId64"/>
+    <hyperlink ref="I14" r:id="rId61"/>
+    <hyperlink ref="G14" r:id="rId62"/>
+    <hyperlink ref="G15" r:id="rId63"/>
+    <hyperlink ref="I15" r:id="rId64"/>
+    <hyperlink ref="G8" r:id="rId65"/>
+    <hyperlink ref="I8" r:id="rId66"/>
+    <hyperlink ref="H8" r:id="rId67"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId65"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId68"/>
   <tableParts count="1">
-    <tablePart r:id="rId66"/>
+    <tablePart r:id="rId69"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add d3d 10 system paper
</commit_message>
<xml_diff>
--- a/reading/readings.xlsx
+++ b/reading/readings.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="200">
   <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -696,6 +696,30 @@
   </si>
   <si>
     <t>https://youtu.be/6b-o_-Xb50E</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/citation.cfm?id=1141947</t>
+  </si>
+  <si>
+    <t>2006年8月</t>
+  </si>
+  <si>
+    <t>SIGGRAPH 2006</t>
+  </si>
+  <si>
+    <t>The Direct3D 10 system</t>
+  </si>
+  <si>
+    <t>David Blythe</t>
+  </si>
+  <si>
+    <t>assets/thumb/dx10.png</t>
+  </si>
+  <si>
+    <t>assets/paper/p724-blythe-d3d10system.pdf</t>
+  </si>
+  <si>
+    <t>D3D 10的Shader Model 4.0是第一个Unified Shader Model</t>
   </si>
 </sst>
 </file>
@@ -848,9 +872,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L20" totalsRowShown="0" headerRowDxfId="10">
-  <sortState ref="A2:L20">
-    <sortCondition descending="1" ref="D2:D20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L21" totalsRowShown="0" headerRowDxfId="10">
+  <sortState ref="A2:L21">
+    <sortCondition descending="1" ref="D2:D21"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" name="title" dataDxfId="9"/>
@@ -1133,11 +1157,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1610,216 +1634,245 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E14" t="s">
+        <v>194</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C15" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D15" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>171</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G15" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I15" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="1" t="s">
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D16" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>178</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G16" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I16" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K16" s="7"/>
-      <c r="L16" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J17" s="7" t="s">
         <v>92</v>
       </c>
       <c r="K17" s="7"/>
       <c r="L17" s="1" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K18" s="7"/>
+      <c r="L18" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D19" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>111</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="E19" t="s">
-        <v>99</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>101</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>103</v>
+        <v>108</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>114</v>
+        <v>96</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>98</v>
       </c>
       <c r="E20" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>101</v>
       </c>
       <c r="G20" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="I20" s="7" t="s">
+      <c r="I21" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1839,9 +1892,9 @@
     <hyperlink ref="G13" r:id="rId11" display="assets\thumb\dod_dice.png"/>
     <hyperlink ref="G7" r:id="rId12" display="assets\thumb\dod_cppcon2014.png"/>
     <hyperlink ref="G4" r:id="rId13" display="assets\thumb\framegraph_gdc2018.png"/>
-    <hyperlink ref="C16" r:id="rId14"/>
-    <hyperlink ref="G16" r:id="rId15" display="assets\thumb\the_rendering_equation.png"/>
-    <hyperlink ref="I16" r:id="rId16" display="assets\paper\p143-kajiya.pdf"/>
+    <hyperlink ref="C17" r:id="rId14"/>
+    <hyperlink ref="G17" r:id="rId15" display="assets\thumb\the_rendering_equation.png"/>
+    <hyperlink ref="I17" r:id="rId16" display="assets\paper\p143-kajiya.pdf"/>
     <hyperlink ref="H5" r:id="rId17"/>
     <hyperlink ref="C5" r:id="rId18"/>
     <hyperlink ref="G5" r:id="rId19" display="assets\thumb\overwatch_ecs_gdc2017.png"/>
@@ -1856,9 +1909,9 @@
     <hyperlink ref="I10" r:id="rId28" display="assets\slides\s2013_pbs_epic_slides.pdf"/>
     <hyperlink ref="J10" r:id="rId29" display="https://neil3d.github.io/unreal/pbr-ue4.html"/>
     <hyperlink ref="K10" r:id="rId30" display="assets\slides\s2013_pbs_epic_notes_v2.pdf"/>
-    <hyperlink ref="C17" r:id="rId31"/>
-    <hyperlink ref="G17" r:id="rId32" display="assets\thumb\cook-brdf.png"/>
-    <hyperlink ref="I17" r:id="rId33" display="assets\paper\p7-cook.pdf"/>
+    <hyperlink ref="C18" r:id="rId31"/>
+    <hyperlink ref="G18" r:id="rId32" display="assets\thumb\cook-brdf.png"/>
+    <hyperlink ref="I18" r:id="rId33" display="assets\paper\p7-cook.pdf"/>
     <hyperlink ref="C2" r:id="rId34"/>
     <hyperlink ref="G2" r:id="rId35" display="assets\thumb\intro_dxr_sig2018.png"/>
     <hyperlink ref="H2" r:id="rId36"/>
@@ -1871,13 +1924,13 @@
     <hyperlink ref="G12" r:id="rId43" display="assets\thumb\disney_pbs_sig2012.png"/>
     <hyperlink ref="I12" r:id="rId44" display="assets\slides\s2012_pbs_disney_brdf_slides_v2.pdf"/>
     <hyperlink ref="K12" r:id="rId45" display="assets\slides\s2012_pbs_disney_brdf_notes_v3.pdf"/>
-    <hyperlink ref="G19" r:id="rId46"/>
-    <hyperlink ref="I19" r:id="rId47"/>
-    <hyperlink ref="I18" r:id="rId48"/>
-    <hyperlink ref="C20" r:id="rId49"/>
-    <hyperlink ref="I20" r:id="rId50"/>
-    <hyperlink ref="G18" r:id="rId51"/>
-    <hyperlink ref="G20" r:id="rId52"/>
+    <hyperlink ref="G20" r:id="rId46"/>
+    <hyperlink ref="I20" r:id="rId47"/>
+    <hyperlink ref="I19" r:id="rId48"/>
+    <hyperlink ref="C21" r:id="rId49"/>
+    <hyperlink ref="I21" r:id="rId50"/>
+    <hyperlink ref="G19" r:id="rId51"/>
+    <hyperlink ref="G21" r:id="rId52"/>
     <hyperlink ref="C9" r:id="rId53"/>
     <hyperlink ref="G9" r:id="rId54"/>
     <hyperlink ref="H9" r:id="rId55"/>
@@ -1886,18 +1939,21 @@
     <hyperlink ref="G6" r:id="rId58"/>
     <hyperlink ref="H6" r:id="rId59"/>
     <hyperlink ref="I6" r:id="rId60"/>
-    <hyperlink ref="I14" r:id="rId61"/>
-    <hyperlink ref="G14" r:id="rId62"/>
-    <hyperlink ref="G15" r:id="rId63"/>
-    <hyperlink ref="I15" r:id="rId64"/>
+    <hyperlink ref="I15" r:id="rId61"/>
+    <hyperlink ref="G15" r:id="rId62"/>
+    <hyperlink ref="G16" r:id="rId63"/>
+    <hyperlink ref="I16" r:id="rId64"/>
     <hyperlink ref="G8" r:id="rId65"/>
     <hyperlink ref="I8" r:id="rId66"/>
     <hyperlink ref="H8" r:id="rId67"/>
+    <hyperlink ref="C14" r:id="rId68"/>
+    <hyperlink ref="G14" r:id="rId69"/>
+    <hyperlink ref="I14" r:id="rId70"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId68"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId71"/>
   <tableParts count="1">
-    <tablePart r:id="rId69"/>
+    <tablePart r:id="rId72"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add gdc vault links
</commit_message>
<xml_diff>
--- a/reading/readings.xlsx
+++ b/reading/readings.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
-  <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neil/work/pages/reading/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="21135"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,13 +16,13 @@
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -244,9 +239,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://www.bilibili.com/video/av10595011/</t>
-  </si>
-  <si>
     <t>PBR Background: Physics and Math of Shading</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -720,23 +712,27 @@
   </si>
   <si>
     <t>D3D 10的Shader Model 4.0是第一个Unified Shader Model</t>
+  </si>
+  <si>
+    <t>https://www.gdcvault.com/play/1024045/FrameGraph-Extensible-Rendering-Architecture-in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -745,7 +741,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -754,7 +750,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -807,8 +803,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -1160,23 +1156,23 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14:XFD14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="23.6640625" style="1" customWidth="1"/>
+    <col min="1" max="3" width="23.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="9" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="20.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="27.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="20.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="27.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1214,45 +1210,45 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="57" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" t="s">
         <v>78</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="J2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:12" ht="57" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1272,23 +1268,23 @@
         <v>20</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K3" s="7"/>
       <c r="L3" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="57" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1308,23 +1304,23 @@
         <v>29</v>
       </c>
       <c r="G4" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>136</v>
-      </c>
       <c r="J4" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
@@ -1344,7 +1340,7 @@
         <v>46</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>44</v>
@@ -1353,52 +1349,52 @@
         <v>50</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" t="s">
         <v>157</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1412,196 +1408,196 @@
         <v>17</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="E8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="E8" t="s">
-        <v>185</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G8" s="7" t="s">
+      <c r="I8" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="I8" s="7" t="s">
+      <c r="L8" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G9" s="7" t="s">
+      <c r="H9" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="7" t="s">
         <v>152</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>153</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="E10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="9" t="s">
+      <c r="E11" t="s">
         <v>57</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="I11" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="J11" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K11" s="7" t="s">
+    </row>
+    <row r="12" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="57" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1621,106 +1617,106 @@
         <v>28</v>
       </c>
       <c r="G13" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="I13" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="J13" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="E14" t="s">
+        <v>193</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="E14" t="s">
-        <v>194</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G14" s="7" t="s">
+      <c r="I14" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="L14" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="E15" t="s">
         <v>170</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>172</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="57" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="D16" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="E16" t="s">
         <v>177</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="I16" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="L16" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
@@ -1737,143 +1733,143 @@
         <v>40</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G17" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I17" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="I17" s="7" t="s">
-        <v>139</v>
-      </c>
       <c r="J17" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K17" s="7"/>
       <c r="L17" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="D18" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="E18" t="s">
         <v>72</v>
       </c>
-      <c r="E18" t="s">
-        <v>73</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G18" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I18" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="I18" s="7" t="s">
-        <v>143</v>
-      </c>
       <c r="J18" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K18" s="7"/>
       <c r="L18" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="E19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="I19" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E19" t="s">
+      <c r="J19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G19" s="7" t="s">
+      <c r="B21" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="E20" t="s">
-        <v>99</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="I21" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="I21" s="7" t="s">
+      <c r="L21" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1949,11 +1945,12 @@
     <hyperlink ref="C14" r:id="rId68"/>
     <hyperlink ref="G14" r:id="rId69"/>
     <hyperlink ref="I14" r:id="rId70"/>
+    <hyperlink ref="H4" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId71"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId72"/>
   <tableParts count="1">
-    <tablePart r:id="rId72"/>
+    <tablePart r:id="rId73"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>